<commit_message>
tile-cased financial legends using pythons awesome title() function
</commit_message>
<xml_diff>
--- a/server/src/static/sudanexample.xlsx
+++ b/server/src/static/sudanexample.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="21240" windowHeight="13305" firstSheet="4" activeTab="6"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="21240" windowHeight="13305" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="1" r:id="rId1"/>
@@ -728,7 +728,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="543" uniqueCount="166">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="543" uniqueCount="167">
   <si>
     <t>* For each parameter (as in, row in the worksheet), there needs to be at least one data point entered. The only exception to this is the sheet "Optional indicators", which may be left blank. If data are not available for a particular indicator, enter an assumption in the "Assumption" column, with a comment explaining how that value was derived.</t>
   </si>
@@ -1015,9 +1015,6 @@
     <t>Monitoring, evaluation, surveillance, and research</t>
   </si>
   <si>
-    <t>PLHIV support</t>
-  </si>
-  <si>
     <t>Cost &amp; coverage</t>
   </si>
   <si>
@@ -1226,6 +1223,12 @@
   </si>
   <si>
     <t>CD4(&gt;500)</t>
+  </si>
+  <si>
+    <t>Other costs</t>
+  </si>
+  <si>
+    <t>Other</t>
   </si>
 </sst>
 </file>
@@ -1948,7 +1951,7 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -2042,7 +2045,7 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
@@ -2136,7 +2139,7 @@
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
@@ -2220,7 +2223,7 @@
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="4" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
@@ -2331,7 +2334,7 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -2413,7 +2416,7 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
@@ -2522,23 +2525,23 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C2" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="D2" s="6" t="s">
         <v>103</v>
       </c>
-      <c r="D2" s="6" t="s">
-        <v>104</v>
-      </c>
       <c r="E2" s="6" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B3" s="5" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C3" s="8">
         <v>4.0000000000000002E-4</v>
@@ -2552,7 +2555,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B4" s="5" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C4" s="8">
         <v>8.0000000000000004E-4</v>
@@ -2566,7 +2569,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B5" s="5" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C5" s="8">
         <v>1.38E-2</v>
@@ -2580,7 +2583,7 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B6" s="5" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C6" s="8">
         <v>1.1000000000000001E-3</v>
@@ -2594,7 +2597,7 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B7" s="5" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C7" s="8">
         <v>8.0000000000000002E-3</v>
@@ -2608,7 +2611,7 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B8" s="5" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C8" s="8">
         <v>0.36699999999999999</v>
@@ -2622,7 +2625,7 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B9" s="5" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C9" s="8">
         <v>0.20499999999999999</v>
@@ -2636,23 +2639,23 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C14" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="D14" s="6" t="s">
         <v>103</v>
       </c>
-      <c r="D14" s="6" t="s">
-        <v>104</v>
-      </c>
       <c r="E14" s="6" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B15" s="5" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C15" s="11">
         <v>26.03</v>
@@ -2666,7 +2669,7 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B16" s="5" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C16" s="11">
         <v>1</v>
@@ -2741,13 +2744,13 @@
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C25" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="D25" s="6" t="s">
         <v>103</v>
       </c>
-      <c r="D25" s="6" t="s">
-        <v>104</v>
-      </c>
       <c r="E25" s="6" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
@@ -2827,13 +2830,13 @@
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C35" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="D35" s="6" t="s">
         <v>103</v>
       </c>
-      <c r="D35" s="6" t="s">
-        <v>104</v>
-      </c>
       <c r="E35" s="6" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
@@ -2899,13 +2902,13 @@
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C44" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="D44" s="6" t="s">
         <v>103</v>
       </c>
-      <c r="D44" s="6" t="s">
-        <v>104</v>
-      </c>
       <c r="E44" s="6" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
@@ -2943,18 +2946,18 @@
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C51" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="D51" s="6" t="s">
         <v>103</v>
       </c>
-      <c r="D51" s="6" t="s">
-        <v>104</v>
-      </c>
       <c r="E51" s="6" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B52" s="5" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C52" s="8">
         <v>3.5999999999999999E-3</v>
@@ -2968,7 +2971,7 @@
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B53" s="5" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C53" s="8">
         <v>3.5999999999999999E-3</v>
@@ -3071,13 +3074,13 @@
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C64" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="D64" s="6" t="s">
         <v>103</v>
       </c>
-      <c r="D64" s="6" t="s">
-        <v>104</v>
-      </c>
       <c r="E64" s="6" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.25">
@@ -3152,7 +3155,7 @@
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B70" s="5" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C70" s="12">
         <v>0.46</v>
@@ -3194,7 +3197,7 @@
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B73" s="5" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C73" s="12">
         <v>0.27500000000000002</v>
@@ -3208,23 +3211,23 @@
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A77" s="4" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C78" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="D78" s="6" t="s">
         <v>103</v>
       </c>
-      <c r="D78" s="6" t="s">
-        <v>104</v>
-      </c>
       <c r="E78" s="6" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B79" s="5" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C79" s="11">
         <v>0.14599999999999999</v>
@@ -3238,7 +3241,7 @@
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B80" s="5" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C80" s="11">
         <v>8.0000000000000002E-3</v>
@@ -3252,7 +3255,7 @@
     </row>
     <row r="81" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B81" s="5" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C81" s="11">
         <v>0.02</v>
@@ -3266,7 +3269,7 @@
     </row>
     <row r="82" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B82" s="5" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C82" s="11">
         <v>7.0000000000000007E-2</v>
@@ -3280,7 +3283,7 @@
     </row>
     <row r="83" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B83" s="5" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C83" s="11">
         <v>0.26500000000000001</v>
@@ -3294,7 +3297,7 @@
     </row>
     <row r="84" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B84" s="5" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C84" s="11">
         <v>0.54700000000000004</v>
@@ -3308,7 +3311,7 @@
     </row>
     <row r="85" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B85" s="5" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C85" s="11">
         <v>5.2999999999999999E-2</v>
@@ -3344,10 +3347,10 @@
   <sheetData>
     <row r="1" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="Y1" s="6" t="s">
         <v>127</v>
-      </c>
-      <c r="Y1" s="6" t="s">
-        <v>128</v>
       </c>
     </row>
     <row r="2" spans="1:27" x14ac:dyDescent="0.25">
@@ -3415,18 +3418,18 @@
         <v>2020</v>
       </c>
       <c r="Y2" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="Z2" s="6" t="s">
         <v>103</v>
       </c>
-      <c r="Z2" s="6" t="s">
-        <v>104</v>
-      </c>
       <c r="AA2" s="6" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="3" spans="1:27" x14ac:dyDescent="0.25">
       <c r="B3" s="6" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C3" s="22">
         <v>41.670326870927902</v>
@@ -3478,7 +3481,7 @@
       <c r="V3" s="10"/>
       <c r="W3" s="10"/>
       <c r="X3" s="9" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="Y3" s="12">
         <v>0.2</v>
@@ -3492,7 +3495,7 @@
     </row>
     <row r="7" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="8" spans="1:27" x14ac:dyDescent="0.25">
@@ -3560,18 +3563,18 @@
         <v>2020</v>
       </c>
       <c r="Y8" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="Z8" s="6" t="s">
         <v>103</v>
       </c>
-      <c r="Z8" s="6" t="s">
-        <v>104</v>
-      </c>
       <c r="AA8" s="6" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="9" spans="1:27" x14ac:dyDescent="0.25">
       <c r="B9" s="6" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C9" s="23">
         <v>0.482758166845627</v>
@@ -3623,7 +3626,7 @@
       <c r="V9" s="10"/>
       <c r="W9" s="10"/>
       <c r="X9" s="9" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="Y9" s="12">
         <v>0.4</v>
@@ -3637,7 +3640,7 @@
     </row>
     <row r="13" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="14" spans="1:27" x14ac:dyDescent="0.25">
@@ -3705,18 +3708,18 @@
         <v>2020</v>
       </c>
       <c r="Y14" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="Z14" s="6" t="s">
         <v>103</v>
       </c>
-      <c r="Z14" s="6" t="s">
-        <v>104</v>
-      </c>
       <c r="AA14" s="6" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="15" spans="1:27" x14ac:dyDescent="0.25">
       <c r="B15" s="6" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C15" s="13">
         <v>12257299147.293604</v>
@@ -3768,7 +3771,7 @@
       <c r="V15" s="10"/>
       <c r="W15" s="10"/>
       <c r="X15" s="9" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="Y15" s="12">
         <v>0.05</v>
@@ -3782,7 +3785,7 @@
     </row>
     <row r="19" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="20" spans="1:27" x14ac:dyDescent="0.25">
@@ -3850,18 +3853,18 @@
         <v>2020</v>
       </c>
       <c r="Y20" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="Z20" s="6" t="s">
         <v>103</v>
       </c>
-      <c r="Z20" s="6" t="s">
-        <v>104</v>
-      </c>
       <c r="AA20" s="6" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="21" spans="1:27" x14ac:dyDescent="0.25">
       <c r="B21" s="6" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C21" s="10"/>
       <c r="D21" s="10"/>
@@ -3885,7 +3888,7 @@
       <c r="V21" s="10"/>
       <c r="W21" s="10"/>
       <c r="X21" s="9" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="Y21" s="10"/>
       <c r="Z21" s="10"/>
@@ -3893,7 +3896,7 @@
     </row>
     <row r="25" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="26" spans="1:27" x14ac:dyDescent="0.25">
@@ -3961,18 +3964,18 @@
         <v>2020</v>
       </c>
       <c r="Y26" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="Z26" s="6" t="s">
         <v>103</v>
       </c>
-      <c r="Z26" s="6" t="s">
-        <v>104</v>
-      </c>
       <c r="AA26" s="6" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="27" spans="1:27" x14ac:dyDescent="0.25">
       <c r="B27" s="6" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C27" s="10"/>
       <c r="D27" s="10"/>
@@ -3996,7 +3999,7 @@
       <c r="V27" s="10"/>
       <c r="W27" s="10"/>
       <c r="X27" s="9" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="Y27" s="10"/>
       <c r="Z27" s="10"/>
@@ -4004,7 +4007,7 @@
     </row>
     <row r="31" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A31" s="4" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="32" spans="1:27" x14ac:dyDescent="0.25">
@@ -4072,18 +4075,18 @@
         <v>2020</v>
       </c>
       <c r="Y32" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="Z32" s="6" t="s">
         <v>103</v>
       </c>
-      <c r="Z32" s="6" t="s">
-        <v>104</v>
-      </c>
       <c r="AA32" s="6" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="33" spans="1:27" x14ac:dyDescent="0.25">
       <c r="B33" s="6" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C33" s="10"/>
       <c r="D33" s="10"/>
@@ -4107,7 +4110,7 @@
       <c r="V33" s="10"/>
       <c r="W33" s="10"/>
       <c r="X33" s="9" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="Y33" s="10"/>
       <c r="Z33" s="10"/>
@@ -4115,7 +4118,7 @@
     </row>
     <row r="37" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A37" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="38" spans="1:27" x14ac:dyDescent="0.25">
@@ -4183,18 +4186,18 @@
         <v>2020</v>
       </c>
       <c r="Y38" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="Z38" s="6" t="s">
         <v>103</v>
       </c>
-      <c r="Z38" s="6" t="s">
-        <v>104</v>
-      </c>
       <c r="AA38" s="6" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="39" spans="1:27" x14ac:dyDescent="0.25">
       <c r="B39" s="6" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C39" s="10"/>
       <c r="D39" s="10"/>
@@ -4218,7 +4221,7 @@
       <c r="V39" s="10"/>
       <c r="W39" s="10"/>
       <c r="X39" s="9" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="Y39" s="10"/>
       <c r="Z39" s="10"/>
@@ -4226,7 +4229,7 @@
     </row>
     <row r="43" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A43" s="4" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="44" spans="1:27" x14ac:dyDescent="0.25">
@@ -4294,18 +4297,18 @@
         <v>2020</v>
       </c>
       <c r="Y44" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="Z44" s="6" t="s">
         <v>103</v>
       </c>
-      <c r="Z44" s="6" t="s">
-        <v>104</v>
-      </c>
       <c r="AA44" s="6" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="45" spans="1:27" x14ac:dyDescent="0.25">
       <c r="B45" s="6" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C45" s="10"/>
       <c r="D45" s="10"/>
@@ -4329,7 +4332,7 @@
       <c r="V45" s="10"/>
       <c r="W45" s="10"/>
       <c r="X45" s="9" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="Y45" s="10"/>
       <c r="Z45" s="10"/>
@@ -4337,7 +4340,7 @@
     </row>
     <row r="49" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A49" s="4" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="50" spans="1:27" x14ac:dyDescent="0.25">
@@ -4405,18 +4408,18 @@
         <v>2020</v>
       </c>
       <c r="Y50" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="Z50" s="6" t="s">
         <v>103</v>
       </c>
-      <c r="Z50" s="6" t="s">
-        <v>104</v>
-      </c>
       <c r="AA50" s="6" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="51" spans="1:27" x14ac:dyDescent="0.25">
       <c r="B51" s="6" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C51" s="10"/>
       <c r="D51" s="10"/>
@@ -4440,7 +4443,7 @@
       <c r="V51" s="10"/>
       <c r="W51" s="10"/>
       <c r="X51" s="9" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="Y51" s="10"/>
       <c r="Z51" s="10"/>
@@ -4448,7 +4451,7 @@
     </row>
     <row r="55" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A55" s="4" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="56" spans="1:27" x14ac:dyDescent="0.25">
@@ -4516,18 +4519,18 @@
         <v>2020</v>
       </c>
       <c r="Y56" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="Z56" s="6" t="s">
         <v>103</v>
       </c>
-      <c r="Z56" s="6" t="s">
-        <v>104</v>
-      </c>
       <c r="AA56" s="6" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="57" spans="1:27" x14ac:dyDescent="0.25">
       <c r="B57" s="6" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C57" s="10"/>
       <c r="D57" s="10"/>
@@ -4551,7 +4554,7 @@
       <c r="V57" s="10"/>
       <c r="W57" s="10"/>
       <c r="X57" s="9" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="Y57" s="10"/>
       <c r="Z57" s="10"/>
@@ -4559,7 +4562,7 @@
     </row>
     <row r="61" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A61" s="4" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="62" spans="1:27" x14ac:dyDescent="0.25">
@@ -4627,18 +4630,18 @@
         <v>2020</v>
       </c>
       <c r="Y62" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="Z62" s="6" t="s">
         <v>103</v>
       </c>
-      <c r="Z62" s="6" t="s">
-        <v>104</v>
-      </c>
       <c r="AA62" s="6" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="63" spans="1:27" x14ac:dyDescent="0.25">
       <c r="B63" s="6" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C63" s="10"/>
       <c r="D63" s="10"/>
@@ -4662,7 +4665,7 @@
       <c r="V63" s="10"/>
       <c r="W63" s="10"/>
       <c r="X63" s="9" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="Y63" s="10"/>
       <c r="Z63" s="10"/>
@@ -4670,7 +4673,7 @@
     </row>
     <row r="67" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A67" s="4" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="68" spans="1:27" x14ac:dyDescent="0.25">
@@ -4738,18 +4741,18 @@
         <v>2020</v>
       </c>
       <c r="Y68" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="Z68" s="6" t="s">
         <v>103</v>
       </c>
-      <c r="Z68" s="6" t="s">
-        <v>104</v>
-      </c>
       <c r="AA68" s="6" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="69" spans="1:27" x14ac:dyDescent="0.25">
       <c r="B69" s="6" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C69" s="10"/>
       <c r="D69" s="10"/>
@@ -4773,7 +4776,7 @@
       <c r="V69" s="10"/>
       <c r="W69" s="10"/>
       <c r="X69" s="9" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="Y69" s="10"/>
       <c r="Z69" s="10"/>
@@ -4781,7 +4784,7 @@
     </row>
     <row r="73" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A73" s="4" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="74" spans="1:27" x14ac:dyDescent="0.25">
@@ -4849,18 +4852,18 @@
         <v>2020</v>
       </c>
       <c r="Y74" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="Z74" s="6" t="s">
         <v>103</v>
       </c>
-      <c r="Z74" s="6" t="s">
-        <v>104</v>
-      </c>
       <c r="AA74" s="6" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="75" spans="1:27" x14ac:dyDescent="0.25">
       <c r="B75" s="6" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C75" s="11"/>
       <c r="D75" s="11"/>
@@ -4886,7 +4889,7 @@
       <c r="V75" s="11"/>
       <c r="W75" s="11"/>
       <c r="X75" s="9" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="Y75" s="24">
         <v>0.03</v>
@@ -4900,7 +4903,7 @@
     </row>
     <row r="76" spans="1:27" x14ac:dyDescent="0.25">
       <c r="B76" s="6" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C76" s="11"/>
       <c r="D76" s="11"/>
@@ -4926,7 +4929,7 @@
       <c r="V76" s="11"/>
       <c r="W76" s="11"/>
       <c r="X76" s="9" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="Y76" s="24">
         <v>0.03</v>
@@ -4966,7 +4969,7 @@
       <c r="V77" s="11"/>
       <c r="W77" s="11"/>
       <c r="X77" s="9" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="Y77" s="24">
         <v>0.03</v>
@@ -5006,7 +5009,7 @@
       <c r="V78" s="11"/>
       <c r="W78" s="11"/>
       <c r="X78" s="9" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="Y78" s="24">
         <v>0.03</v>
@@ -5046,7 +5049,7 @@
       <c r="V79" s="11"/>
       <c r="W79" s="11"/>
       <c r="X79" s="9" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="Y79" s="24">
         <v>0.03</v>
@@ -5086,7 +5089,7 @@
       <c r="V80" s="11"/>
       <c r="W80" s="11"/>
       <c r="X80" s="9" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="Y80" s="24">
         <v>0.03</v>
@@ -5109,7 +5112,7 @@
     </row>
     <row r="84" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A84" s="4" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="Y84" s="25"/>
     </row>
@@ -5178,18 +5181,18 @@
         <v>2020</v>
       </c>
       <c r="Y85" s="26" t="s">
+        <v>102</v>
+      </c>
+      <c r="Z85" s="26" t="s">
         <v>103</v>
       </c>
-      <c r="Z85" s="26" t="s">
-        <v>104</v>
-      </c>
       <c r="AA85" s="26" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="86" spans="1:27" x14ac:dyDescent="0.25">
       <c r="B86" s="6" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C86" s="11"/>
       <c r="D86" s="11"/>
@@ -5215,7 +5218,7 @@
       <c r="V86" s="11"/>
       <c r="W86" s="11"/>
       <c r="X86" s="9" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="Y86" s="24">
         <v>0.03</v>
@@ -5229,7 +5232,7 @@
     </row>
     <row r="87" spans="1:27" x14ac:dyDescent="0.25">
       <c r="B87" s="6" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C87" s="11"/>
       <c r="D87" s="11"/>
@@ -5255,7 +5258,7 @@
       <c r="V87" s="11"/>
       <c r="W87" s="11"/>
       <c r="X87" s="9" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="Y87" s="24">
         <v>0.03</v>
@@ -5295,7 +5298,7 @@
       <c r="V88" s="11"/>
       <c r="W88" s="11"/>
       <c r="X88" s="9" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="Y88" s="24">
         <v>0.03</v>
@@ -5335,7 +5338,7 @@
       <c r="V89" s="11"/>
       <c r="W89" s="11"/>
       <c r="X89" s="9" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="Y89" s="24">
         <v>0.03</v>
@@ -5375,7 +5378,7 @@
       <c r="V90" s="11"/>
       <c r="W90" s="11"/>
       <c r="X90" s="9" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="Y90" s="24">
         <v>0.03</v>
@@ -5415,7 +5418,7 @@
       <c r="V91" s="11"/>
       <c r="W91" s="11"/>
       <c r="X91" s="9" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="Y91" s="24">
         <v>0.03</v>
@@ -5443,7 +5446,9 @@
   <sheetPr published="0" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:K21"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D20" sqref="D20"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -5754,10 +5759,10 @@
         <v>9</v>
       </c>
       <c r="C21" s="7" t="s">
-        <v>95</v>
+        <v>166</v>
       </c>
       <c r="D21" s="7" t="s">
-        <v>95</v>
+        <v>165</v>
       </c>
     </row>
   </sheetData>
@@ -5787,7 +5792,7 @@
   <sheetData>
     <row r="1" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="2" spans="1:26" x14ac:dyDescent="0.25">
@@ -5855,7 +5860,7 @@
         <v>2020</v>
       </c>
       <c r="Z2" s="6" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="3" spans="1:26" x14ac:dyDescent="0.25">
@@ -5864,7 +5869,7 @@
         <v>SBCC</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D3" s="8"/>
       <c r="E3" s="8"/>
@@ -5890,7 +5895,7 @@
       <c r="W3" s="8"/>
       <c r="X3" s="8"/>
       <c r="Y3" s="9" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="Z3" s="8"/>
     </row>
@@ -5900,7 +5905,7 @@
         <v>SBCC</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
@@ -5926,7 +5931,7 @@
       <c r="W4" s="10"/>
       <c r="X4" s="10"/>
       <c r="Y4" s="9" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="Z4" s="10"/>
     </row>
@@ -5936,7 +5941,7 @@
         <v>FSW programs</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D6" s="8"/>
       <c r="E6" s="8"/>
@@ -5962,7 +5967,7 @@
       <c r="W6" s="8"/>
       <c r="X6" s="8"/>
       <c r="Y6" s="9" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="Z6" s="8"/>
     </row>
@@ -5972,7 +5977,7 @@
         <v>FSW programs</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D7" s="10"/>
       <c r="E7" s="10"/>
@@ -5998,7 +6003,7 @@
       <c r="W7" s="10"/>
       <c r="X7" s="10"/>
       <c r="Y7" s="9" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="Z7" s="10"/>
     </row>
@@ -6008,7 +6013,7 @@
         <v>MSM programs</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D9" s="8"/>
       <c r="E9" s="8"/>
@@ -6034,7 +6039,7 @@
       <c r="W9" s="8"/>
       <c r="X9" s="8"/>
       <c r="Y9" s="9" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="Z9" s="8"/>
     </row>
@@ -6044,7 +6049,7 @@
         <v>MSM programs</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D10" s="10"/>
       <c r="E10" s="10"/>
@@ -6070,7 +6075,7 @@
       <c r="W10" s="10"/>
       <c r="X10" s="10"/>
       <c r="Y10" s="9" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="Z10" s="10"/>
     </row>
@@ -6080,7 +6085,7 @@
         <v>HTC</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D12" s="8"/>
       <c r="E12" s="8"/>
@@ -6106,7 +6111,7 @@
       <c r="W12" s="8"/>
       <c r="X12" s="8"/>
       <c r="Y12" s="9" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="Z12" s="8"/>
     </row>
@@ -6116,7 +6121,7 @@
         <v>HTC</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D13" s="10"/>
       <c r="E13" s="10"/>
@@ -6142,7 +6147,7 @@
       <c r="W13" s="10"/>
       <c r="X13" s="10"/>
       <c r="Y13" s="9" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="Z13" s="10"/>
     </row>
@@ -6152,7 +6157,7 @@
         <v>ART</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D15" s="8"/>
       <c r="E15" s="8"/>
@@ -6178,7 +6183,7 @@
       <c r="W15" s="8"/>
       <c r="X15" s="8"/>
       <c r="Y15" s="9" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="Z15" s="8"/>
     </row>
@@ -6188,7 +6193,7 @@
         <v>ART</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
@@ -6214,7 +6219,7 @@
       <c r="W16" s="10"/>
       <c r="X16" s="10"/>
       <c r="Y16" s="9" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="Z16" s="10"/>
     </row>
@@ -6224,7 +6229,7 @@
         <v>PMTCT</v>
       </c>
       <c r="C18" s="6" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D18" s="8"/>
       <c r="E18" s="8"/>
@@ -6250,7 +6255,7 @@
       <c r="W18" s="8"/>
       <c r="X18" s="8"/>
       <c r="Y18" s="9" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="Z18" s="8"/>
     </row>
@@ -6260,7 +6265,7 @@
         <v>PMTCT</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D19" s="10"/>
       <c r="E19" s="10"/>
@@ -6286,7 +6291,7 @@
       <c r="W19" s="10"/>
       <c r="X19" s="10"/>
       <c r="Y19" s="9" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="Z19" s="10"/>
     </row>
@@ -6296,7 +6301,7 @@
         <v>MGMT</v>
       </c>
       <c r="C21" s="6" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D21" s="8"/>
       <c r="E21" s="8"/>
@@ -6320,7 +6325,7 @@
       <c r="W21" s="8"/>
       <c r="X21" s="8"/>
       <c r="Y21" s="9" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="Z21" s="8"/>
     </row>
@@ -6330,7 +6335,7 @@
         <v>MGMT</v>
       </c>
       <c r="C22" s="6" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D22" s="10"/>
       <c r="E22" s="10"/>
@@ -6356,7 +6361,7 @@
       <c r="W22" s="10"/>
       <c r="X22" s="10"/>
       <c r="Y22" s="9" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="Z22" s="10"/>
     </row>
@@ -6366,7 +6371,7 @@
         <v>M&amp;E</v>
       </c>
       <c r="C24" s="6" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D24" s="8"/>
       <c r="E24" s="8"/>
@@ -6390,7 +6395,7 @@
       <c r="W24" s="8"/>
       <c r="X24" s="8"/>
       <c r="Y24" s="9" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="Z24" s="8"/>
     </row>
@@ -6400,7 +6405,7 @@
         <v>M&amp;E</v>
       </c>
       <c r="C25" s="6" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D25" s="10"/>
       <c r="E25" s="10"/>
@@ -6426,17 +6431,17 @@
       <c r="W25" s="10"/>
       <c r="X25" s="10"/>
       <c r="Y25" s="9" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="Z25" s="10"/>
     </row>
     <row r="27" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B27" s="6" t="str">
         <f>'Populations &amp; programs'!$C$21</f>
-        <v>PLHIV support</v>
+        <v>Other</v>
       </c>
       <c r="C27" s="6" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D27" s="8"/>
       <c r="E27" s="8"/>
@@ -6460,17 +6465,17 @@
       <c r="W27" s="8"/>
       <c r="X27" s="8"/>
       <c r="Y27" s="9" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="Z27" s="8"/>
     </row>
     <row r="28" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B28" s="6" t="str">
         <f>'Populations &amp; programs'!$C$21</f>
-        <v>PLHIV support</v>
+        <v>Other</v>
       </c>
       <c r="C28" s="6" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D28" s="10"/>
       <c r="E28" s="10"/>
@@ -6496,7 +6501,7 @@
       <c r="W28" s="10"/>
       <c r="X28" s="10"/>
       <c r="Y28" s="9" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="Z28" s="10"/>
     </row>
@@ -6525,7 +6530,7 @@
   <sheetData>
     <row r="1" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="2" spans="1:26" x14ac:dyDescent="0.25">
@@ -6593,7 +6598,7 @@
         <v>2020</v>
       </c>
       <c r="Z2" s="6" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="3" spans="1:26" x14ac:dyDescent="0.25">
@@ -6602,7 +6607,7 @@
         <v>FSW</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D3" s="10"/>
       <c r="E3" s="10"/>
@@ -6626,7 +6631,7 @@
       <c r="W3" s="10"/>
       <c r="X3" s="10"/>
       <c r="Y3" s="9" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="Z3" s="10"/>
     </row>
@@ -6636,7 +6641,7 @@
         <v>FSW</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D4" s="13">
         <v>139172.68199999997</v>
@@ -6682,7 +6687,7 @@
       <c r="W4" s="10"/>
       <c r="X4" s="10"/>
       <c r="Y4" s="9" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="Z4" s="10"/>
     </row>
@@ -6692,7 +6697,7 @@
         <v>FSW</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D5" s="10"/>
       <c r="E5" s="10"/>
@@ -6716,7 +6721,7 @@
       <c r="W5" s="10"/>
       <c r="X5" s="10"/>
       <c r="Y5" s="9" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="Z5" s="10"/>
     </row>
@@ -6726,7 +6731,7 @@
         <v>Clients</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D7" s="10"/>
       <c r="E7" s="10"/>
@@ -6750,7 +6755,7 @@
       <c r="W7" s="10"/>
       <c r="X7" s="10"/>
       <c r="Y7" s="9" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="Z7" s="10"/>
     </row>
@@ -6760,7 +6765,7 @@
         <v>Clients</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D8" s="13">
         <v>979330.74050000007</v>
@@ -6806,7 +6811,7 @@
       <c r="W8" s="10"/>
       <c r="X8" s="10"/>
       <c r="Y8" s="9" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="Z8" s="10"/>
     </row>
@@ -6816,7 +6821,7 @@
         <v>Clients</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D9" s="10"/>
       <c r="E9" s="10"/>
@@ -6840,7 +6845,7 @@
       <c r="W9" s="10"/>
       <c r="X9" s="10"/>
       <c r="Y9" s="9" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="Z9" s="10"/>
     </row>
@@ -6850,7 +6855,7 @@
         <v>MSM</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D11" s="10"/>
       <c r="E11" s="10"/>
@@ -6874,7 +6879,7 @@
       <c r="W11" s="10"/>
       <c r="X11" s="10"/>
       <c r="Y11" s="9" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="Z11" s="10"/>
     </row>
@@ -6884,7 +6889,7 @@
         <v>MSM</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D12" s="13">
         <v>96306.278800000015</v>
@@ -6930,7 +6935,7 @@
       <c r="W12" s="10"/>
       <c r="X12" s="10"/>
       <c r="Y12" s="9" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="Z12" s="10"/>
     </row>
@@ -6940,7 +6945,7 @@
         <v>MSM</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D13" s="10"/>
       <c r="E13" s="10"/>
@@ -6964,7 +6969,7 @@
       <c r="W13" s="10"/>
       <c r="X13" s="10"/>
       <c r="Y13" s="9" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="Z13" s="10"/>
     </row>
@@ -6974,7 +6979,7 @@
         <v>Males 15-49</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D15" s="10"/>
       <c r="E15" s="10"/>
@@ -6998,7 +7003,7 @@
       <c r="W15" s="10"/>
       <c r="X15" s="10"/>
       <c r="Y15" s="9" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="Z15" s="10"/>
     </row>
@@ -7008,7 +7013,7 @@
         <v>Males 15-49</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D16" s="10">
         <v>5431543.9807000002</v>
@@ -7054,7 +7059,7 @@
       <c r="W16" s="10"/>
       <c r="X16" s="10"/>
       <c r="Y16" s="9" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="Z16" s="10"/>
     </row>
@@ -7064,7 +7069,7 @@
         <v>Males 15-49</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
@@ -7088,7 +7093,7 @@
       <c r="W17" s="10"/>
       <c r="X17" s="10"/>
       <c r="Y17" s="9" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="Z17" s="10"/>
     </row>
@@ -7098,7 +7103,7 @@
         <v>Females 15-49</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D19" s="10"/>
       <c r="E19" s="10"/>
@@ -7122,7 +7127,7 @@
       <c r="W19" s="10"/>
       <c r="X19" s="10"/>
       <c r="Y19" s="9" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="Z19" s="10"/>
     </row>
@@ -7132,7 +7137,7 @@
         <v>Females 15-49</v>
       </c>
       <c r="C20" s="6" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D20" s="10">
         <v>6333671.4559585694</v>
@@ -7178,7 +7183,7 @@
       <c r="W20" s="10"/>
       <c r="X20" s="10"/>
       <c r="Y20" s="9" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="Z20" s="10"/>
     </row>
@@ -7188,7 +7193,7 @@
         <v>Females 15-49</v>
       </c>
       <c r="C21" s="6" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D21" s="10"/>
       <c r="E21" s="10"/>
@@ -7212,13 +7217,13 @@
       <c r="W21" s="10"/>
       <c r="X21" s="10"/>
       <c r="Y21" s="9" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="Z21" s="10"/>
     </row>
     <row r="26" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="27" spans="1:26" x14ac:dyDescent="0.25">
@@ -7286,7 +7291,7 @@
         <v>2020</v>
       </c>
       <c r="Z27" s="6" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="28" spans="1:26" x14ac:dyDescent="0.25">
@@ -7295,7 +7300,7 @@
         <v>FSW</v>
       </c>
       <c r="C28" s="6" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D28" s="8"/>
       <c r="E28" s="8"/>
@@ -7319,7 +7324,7 @@
       <c r="W28" s="8"/>
       <c r="X28" s="8"/>
       <c r="Y28" s="9" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="Z28" s="8"/>
     </row>
@@ -7329,7 +7334,7 @@
         <v>FSW</v>
       </c>
       <c r="C29" s="6" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D29" s="8"/>
       <c r="E29" s="8"/>
@@ -7355,7 +7360,7 @@
       <c r="W29" s="8"/>
       <c r="X29" s="8"/>
       <c r="Y29" s="9" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="Z29" s="8"/>
     </row>
@@ -7365,7 +7370,7 @@
         <v>FSW</v>
       </c>
       <c r="C30" s="6" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D30" s="8"/>
       <c r="E30" s="8"/>
@@ -7389,7 +7394,7 @@
       <c r="W30" s="8"/>
       <c r="X30" s="8"/>
       <c r="Y30" s="9" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="Z30" s="8"/>
     </row>
@@ -7399,7 +7404,7 @@
         <v>Clients</v>
       </c>
       <c r="C32" s="6" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D32" s="8"/>
       <c r="E32" s="8"/>
@@ -7423,7 +7428,7 @@
       <c r="W32" s="8"/>
       <c r="X32" s="8"/>
       <c r="Y32" s="9" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="Z32" s="8"/>
     </row>
@@ -7433,7 +7438,7 @@
         <v>Clients</v>
       </c>
       <c r="C33" s="6" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D33" s="8"/>
       <c r="E33" s="8"/>
@@ -7459,7 +7464,7 @@
       <c r="W33" s="8"/>
       <c r="X33" s="8"/>
       <c r="Y33" s="9" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="Z33" s="8"/>
     </row>
@@ -7469,7 +7474,7 @@
         <v>Clients</v>
       </c>
       <c r="C34" s="6" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D34" s="8"/>
       <c r="E34" s="8"/>
@@ -7493,7 +7498,7 @@
       <c r="W34" s="8"/>
       <c r="X34" s="8"/>
       <c r="Y34" s="9" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="Z34" s="8"/>
     </row>
@@ -7503,7 +7508,7 @@
         <v>MSM</v>
       </c>
       <c r="C36" s="6" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D36" s="8"/>
       <c r="E36" s="8"/>
@@ -7527,7 +7532,7 @@
       <c r="W36" s="8"/>
       <c r="X36" s="8"/>
       <c r="Y36" s="9" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="Z36" s="8"/>
     </row>
@@ -7537,7 +7542,7 @@
         <v>MSM</v>
       </c>
       <c r="C37" s="6" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D37" s="8"/>
       <c r="E37" s="8"/>
@@ -7563,7 +7568,7 @@
       <c r="W37" s="8"/>
       <c r="X37" s="8"/>
       <c r="Y37" s="9" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="Z37" s="8"/>
     </row>
@@ -7573,7 +7578,7 @@
         <v>MSM</v>
       </c>
       <c r="C38" s="6" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D38" s="8"/>
       <c r="E38" s="8"/>
@@ -7597,7 +7602,7 @@
       <c r="W38" s="8"/>
       <c r="X38" s="8"/>
       <c r="Y38" s="9" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="Z38" s="8"/>
     </row>
@@ -7607,7 +7612,7 @@
         <v>Males 15-49</v>
       </c>
       <c r="C40" s="6" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D40" s="8"/>
       <c r="E40" s="8"/>
@@ -7631,7 +7636,7 @@
       <c r="W40" s="8"/>
       <c r="X40" s="8"/>
       <c r="Y40" s="9" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="Z40" s="8"/>
     </row>
@@ -7641,7 +7646,7 @@
         <v>Males 15-49</v>
       </c>
       <c r="C41" s="6" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D41" s="8"/>
       <c r="E41" s="8"/>
@@ -7671,7 +7676,7 @@
       <c r="W41" s="8"/>
       <c r="X41" s="8"/>
       <c r="Y41" s="9" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="Z41" s="8"/>
     </row>
@@ -7681,7 +7686,7 @@
         <v>Males 15-49</v>
       </c>
       <c r="C42" s="6" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D42" s="8"/>
       <c r="E42" s="8"/>
@@ -7705,7 +7710,7 @@
       <c r="W42" s="8"/>
       <c r="X42" s="8"/>
       <c r="Y42" s="9" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="Z42" s="8"/>
     </row>
@@ -7715,7 +7720,7 @@
         <v>Females 15-49</v>
       </c>
       <c r="C44" s="6" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D44" s="8"/>
       <c r="E44" s="8"/>
@@ -7739,7 +7744,7 @@
       <c r="W44" s="8"/>
       <c r="X44" s="8"/>
       <c r="Y44" s="9" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="Z44" s="8"/>
     </row>
@@ -7749,7 +7754,7 @@
         <v>Females 15-49</v>
       </c>
       <c r="C45" s="6" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D45" s="8"/>
       <c r="E45" s="8"/>
@@ -7779,7 +7784,7 @@
       <c r="W45" s="8"/>
       <c r="X45" s="8"/>
       <c r="Y45" s="9" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="Z45" s="8"/>
     </row>
@@ -7789,7 +7794,7 @@
         <v>Females 15-49</v>
       </c>
       <c r="C46" s="6" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D46" s="8"/>
       <c r="E46" s="8"/>
@@ -7813,7 +7818,7 @@
       <c r="W46" s="8"/>
       <c r="X46" s="8"/>
       <c r="Y46" s="9" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="Z46" s="8"/>
     </row>
@@ -7842,7 +7847,7 @@
   <sheetData>
     <row r="1" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="2" spans="1:25" x14ac:dyDescent="0.25">
@@ -7910,12 +7915,12 @@
         <v>2020</v>
       </c>
       <c r="Y2" s="6" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="3" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B3" s="6" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C3" s="11"/>
       <c r="D3" s="11"/>
@@ -7953,13 +7958,13 @@
       <c r="V3" s="11"/>
       <c r="W3" s="11"/>
       <c r="X3" s="9" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="Y3" s="11"/>
     </row>
     <row r="7" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="8" spans="1:25" x14ac:dyDescent="0.25">
@@ -8027,12 +8032,12 @@
         <v>2020</v>
       </c>
       <c r="Y8" s="6" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="9" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B9" s="6" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C9" s="11"/>
       <c r="D9" s="11"/>
@@ -8058,13 +8063,13 @@
       <c r="V9" s="11"/>
       <c r="W9" s="11"/>
       <c r="X9" s="9" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="Y9" s="11"/>
     </row>
     <row r="13" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="14" spans="1:25" x14ac:dyDescent="0.25">
@@ -8132,12 +8137,12 @@
         <v>2020</v>
       </c>
       <c r="Y14" s="6" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="15" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B15" s="6" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C15" s="16">
         <v>3121.27</v>
@@ -8189,13 +8194,13 @@
       <c r="V15" s="11"/>
       <c r="W15" s="11"/>
       <c r="X15" s="9" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="Y15" s="11"/>
     </row>
     <row r="19" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="20" spans="1:25" x14ac:dyDescent="0.25">
@@ -8263,12 +8268,12 @@
         <v>2020</v>
       </c>
       <c r="Y20" s="6" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="21" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B21" s="6" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C21" s="11">
         <v>0.11</v>
@@ -8320,13 +8325,13 @@
       <c r="V21" s="11"/>
       <c r="W21" s="11"/>
       <c r="X21" s="9" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="Y21" s="11"/>
     </row>
     <row r="25" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="26" spans="1:25" x14ac:dyDescent="0.25">
@@ -8394,12 +8399,12 @@
         <v>2020</v>
       </c>
       <c r="Y26" s="6" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="27" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B27" s="6" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C27" s="16">
         <v>714</v>
@@ -8451,13 +8456,13 @@
       <c r="V27" s="11"/>
       <c r="W27" s="11"/>
       <c r="X27" s="9" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="Y27" s="11"/>
     </row>
     <row r="31" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A31" s="4" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="32" spans="1:25" x14ac:dyDescent="0.25">
@@ -8525,12 +8530,12 @@
         <v>2020</v>
       </c>
       <c r="Y32" s="6" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="33" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B33" s="6" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C33" s="11"/>
       <c r="D33" s="11"/>
@@ -8554,7 +8559,7 @@
       <c r="V33" s="11"/>
       <c r="W33" s="11"/>
       <c r="X33" s="9" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="Y33" s="11"/>
     </row>
@@ -8583,7 +8588,7 @@
   <sheetData>
     <row r="1" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="2" spans="1:25" x14ac:dyDescent="0.25">
@@ -8651,7 +8656,7 @@
         <v>2020</v>
       </c>
       <c r="Y2" s="6" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="3" spans="1:25" x14ac:dyDescent="0.25">
@@ -8681,7 +8686,7 @@
       <c r="V3" s="8"/>
       <c r="W3" s="8"/>
       <c r="X3" s="9" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="Y3" s="8">
         <v>0.01</v>
@@ -8714,7 +8719,7 @@
       <c r="V4" s="8"/>
       <c r="W4" s="8"/>
       <c r="X4" s="9" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="Y4" s="8">
         <v>0.01</v>
@@ -8747,7 +8752,7 @@
       <c r="V5" s="8"/>
       <c r="W5" s="8"/>
       <c r="X5" s="9" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="Y5" s="8">
         <v>0.01</v>
@@ -8780,7 +8785,7 @@
       <c r="V6" s="8"/>
       <c r="W6" s="8"/>
       <c r="X6" s="9" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="Y6" s="8">
         <v>0.01</v>
@@ -8813,7 +8818,7 @@
       <c r="V7" s="8"/>
       <c r="W7" s="8"/>
       <c r="X7" s="9" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="Y7" s="8">
         <v>0.01</v>
@@ -8821,7 +8826,7 @@
     </row>
     <row r="11" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="12" spans="1:25" x14ac:dyDescent="0.25">
@@ -8889,7 +8894,7 @@
         <v>2020</v>
       </c>
       <c r="Y12" s="6" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="13" spans="1:25" x14ac:dyDescent="0.25">
@@ -8921,7 +8926,7 @@
       <c r="V13" s="8"/>
       <c r="W13" s="8"/>
       <c r="X13" s="9" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="Y13" s="8"/>
     </row>
@@ -8952,7 +8957,7 @@
       <c r="V14" s="8"/>
       <c r="W14" s="8"/>
       <c r="X14" s="9" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="Y14" s="8">
         <v>0.02</v>
@@ -8987,7 +8992,7 @@
       <c r="V15" s="8"/>
       <c r="W15" s="8"/>
       <c r="X15" s="9" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="Y15" s="8"/>
     </row>
@@ -9018,7 +9023,7 @@
       <c r="V16" s="8"/>
       <c r="W16" s="8"/>
       <c r="X16" s="9" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="Y16" s="8">
         <v>0.01</v>
@@ -9051,7 +9056,7 @@
       <c r="V17" s="8"/>
       <c r="W17" s="8"/>
       <c r="X17" s="9" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="Y17" s="8">
         <v>0.01</v>
@@ -9059,7 +9064,7 @@
     </row>
     <row r="21" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="22" spans="1:25" x14ac:dyDescent="0.25">
@@ -9127,7 +9132,7 @@
         <v>2020</v>
       </c>
       <c r="Y22" s="6" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="23" spans="1:25" x14ac:dyDescent="0.25">
@@ -9159,7 +9164,7 @@
       <c r="V23" s="8"/>
       <c r="W23" s="8"/>
       <c r="X23" s="9" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="Y23" s="8"/>
     </row>
@@ -9190,7 +9195,7 @@
       <c r="V24" s="8"/>
       <c r="W24" s="8"/>
       <c r="X24" s="9" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="Y24" s="8">
         <v>0.05</v>
@@ -9225,7 +9230,7 @@
       <c r="V25" s="8"/>
       <c r="W25" s="8"/>
       <c r="X25" s="9" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="Y25" s="8"/>
     </row>
@@ -9256,7 +9261,7 @@
       <c r="V26" s="8"/>
       <c r="W26" s="8"/>
       <c r="X26" s="9" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="Y26" s="8">
         <v>0.01</v>
@@ -9289,7 +9294,7 @@
       <c r="V27" s="8"/>
       <c r="W27" s="8"/>
       <c r="X27" s="9" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="Y27" s="8">
         <v>0.02</v>
@@ -9297,7 +9302,7 @@
     </row>
     <row r="31" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A31" s="4" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="32" spans="1:25" x14ac:dyDescent="0.25">
@@ -9365,7 +9370,7 @@
         <v>2020</v>
       </c>
       <c r="Y32" s="6" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="33" spans="2:25" x14ac:dyDescent="0.25">
@@ -9398,7 +9403,7 @@
       <c r="V33" s="8"/>
       <c r="W33" s="8"/>
       <c r="X33" s="9" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="Y33" s="8"/>
     </row>
@@ -9432,7 +9437,7 @@
       <c r="V34" s="8"/>
       <c r="W34" s="8"/>
       <c r="X34" s="9" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="Y34" s="8"/>
     </row>
@@ -9466,7 +9471,7 @@
       <c r="V35" s="8"/>
       <c r="W35" s="8"/>
       <c r="X35" s="9" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="Y35" s="8"/>
     </row>
@@ -9500,7 +9505,7 @@
       <c r="V36" s="8"/>
       <c r="W36" s="8"/>
       <c r="X36" s="9" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="Y36" s="8"/>
     </row>
@@ -9534,7 +9539,7 @@
       <c r="V37" s="8"/>
       <c r="W37" s="8"/>
       <c r="X37" s="9" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="Y37" s="8"/>
     </row>
@@ -9555,7 +9560,7 @@
   <sheetPr published="0" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:Y60"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="Q28" sqref="Q28"/>
     </sheetView>
   </sheetViews>
@@ -9631,7 +9636,7 @@
         <v>2020</v>
       </c>
       <c r="Y2" s="6" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="3" spans="1:25" x14ac:dyDescent="0.25">
@@ -9665,7 +9670,7 @@
       <c r="V3" s="12"/>
       <c r="W3" s="12"/>
       <c r="X3" s="9" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="Y3" s="12"/>
     </row>
@@ -9698,7 +9703,7 @@
       <c r="V4" s="12"/>
       <c r="W4" s="12"/>
       <c r="X4" s="9" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="Y4" s="12"/>
     </row>
@@ -9731,7 +9736,7 @@
       <c r="V5" s="12"/>
       <c r="W5" s="12"/>
       <c r="X5" s="9" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="Y5" s="12"/>
     </row>
@@ -9764,7 +9769,7 @@
       <c r="V6" s="12"/>
       <c r="W6" s="12"/>
       <c r="X6" s="9" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="Y6" s="12"/>
     </row>
@@ -9797,7 +9802,7 @@
       <c r="V7" s="12"/>
       <c r="W7" s="12"/>
       <c r="X7" s="9" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="Y7" s="12"/>
     </row>
@@ -9871,7 +9876,7 @@
         <v>2020</v>
       </c>
       <c r="Y12" s="6" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="13" spans="1:25" x14ac:dyDescent="0.25">
@@ -9902,7 +9907,7 @@
       <c r="V13" s="7"/>
       <c r="W13" s="7"/>
       <c r="X13" s="9" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="Y13" s="7"/>
     </row>
@@ -9976,12 +9981,12 @@
         <v>2020</v>
       </c>
       <c r="Y18" s="6" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="19" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B19" s="6" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C19" s="7"/>
       <c r="D19" s="7"/>
@@ -10017,7 +10022,7 @@
       <c r="V19" s="7"/>
       <c r="W19" s="7"/>
       <c r="X19" s="9" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="Y19" s="7"/>
     </row>
@@ -10091,12 +10096,12 @@
         <v>2020</v>
       </c>
       <c r="Y24" s="6" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="25" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B25" s="6" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C25" s="7"/>
       <c r="D25" s="7"/>
@@ -10132,7 +10137,7 @@
       <c r="V25" s="7"/>
       <c r="W25" s="7"/>
       <c r="X25" s="9" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="Y25" s="7"/>
     </row>
@@ -10206,12 +10211,12 @@
         <v>2020</v>
       </c>
       <c r="Y30" s="6" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="31" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B31" s="6" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C31" s="7"/>
       <c r="D31" s="7"/>
@@ -10257,7 +10262,7 @@
       <c r="V31" s="7"/>
       <c r="W31" s="7"/>
       <c r="X31" s="9" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="Y31" s="7"/>
     </row>
@@ -10331,7 +10336,7 @@
         <v>2020</v>
       </c>
       <c r="Y36" s="6" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="37" spans="1:25" x14ac:dyDescent="0.25">
@@ -10361,7 +10366,7 @@
       <c r="V37" s="12"/>
       <c r="W37" s="12"/>
       <c r="X37" s="9" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="Y37" s="12">
         <v>0</v>
@@ -10394,7 +10399,7 @@
       <c r="V38" s="12"/>
       <c r="W38" s="12"/>
       <c r="X38" s="9" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="Y38" s="12">
         <v>0</v>
@@ -10427,7 +10432,7 @@
       <c r="V39" s="12"/>
       <c r="W39" s="12"/>
       <c r="X39" s="9" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="Y39" s="12">
         <v>0</v>
@@ -10460,7 +10465,7 @@
       <c r="V40" s="12"/>
       <c r="W40" s="12"/>
       <c r="X40" s="9" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="Y40" s="12">
         <v>0</v>
@@ -10493,7 +10498,7 @@
       <c r="V41" s="12"/>
       <c r="W41" s="12"/>
       <c r="X41" s="9" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="Y41" s="12">
         <v>0</v>
@@ -10569,12 +10574,12 @@
         <v>2020</v>
       </c>
       <c r="Y46" s="6" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="47" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B47" s="6" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C47" s="7"/>
       <c r="D47" s="7"/>
@@ -10602,7 +10607,7 @@
       <c r="V47" s="7"/>
       <c r="W47" s="7"/>
       <c r="X47" s="9" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="Y47" s="7"/>
     </row>
@@ -10676,7 +10681,7 @@
         <v>2020</v>
       </c>
       <c r="Y52" s="6" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="53" spans="1:25" x14ac:dyDescent="0.25">
@@ -10734,7 +10739,7 @@
       <c r="V53" s="11"/>
       <c r="W53" s="11"/>
       <c r="X53" s="9" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="Y53" s="11"/>
     </row>
@@ -10793,7 +10798,7 @@
       <c r="V54" s="11"/>
       <c r="W54" s="11"/>
       <c r="X54" s="9" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="Y54" s="11"/>
     </row>
@@ -10867,12 +10872,12 @@
         <v>2020</v>
       </c>
       <c r="Y59" s="6" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="60" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B60" s="6" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C60" s="12"/>
       <c r="D60" s="12"/>
@@ -10898,7 +10903,7 @@
       <c r="V60" s="12"/>
       <c r="W60" s="12"/>
       <c r="X60" s="9" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="Y60" s="12"/>
     </row>
@@ -10995,7 +11000,7 @@
         <v>2020</v>
       </c>
       <c r="Y2" s="6" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="3" spans="1:25" x14ac:dyDescent="0.25">
@@ -11027,7 +11032,7 @@
       <c r="V3" s="7"/>
       <c r="W3" s="7"/>
       <c r="X3" s="9" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="Y3" s="7"/>
     </row>
@@ -11060,7 +11065,7 @@
       <c r="V4" s="7"/>
       <c r="W4" s="7"/>
       <c r="X4" s="9" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="Y4" s="7"/>
     </row>
@@ -11093,7 +11098,7 @@
       <c r="V5" s="7"/>
       <c r="W5" s="7"/>
       <c r="X5" s="9" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="Y5" s="7"/>
     </row>
@@ -11126,7 +11131,7 @@
       <c r="V6" s="7"/>
       <c r="W6" s="7"/>
       <c r="X6" s="9" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="Y6" s="7"/>
     </row>
@@ -11159,7 +11164,7 @@
       <c r="V7" s="7"/>
       <c r="W7" s="7"/>
       <c r="X7" s="9" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="Y7" s="7"/>
     </row>
@@ -11233,7 +11238,7 @@
         <v>2020</v>
       </c>
       <c r="Y12" s="6" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="13" spans="1:25" x14ac:dyDescent="0.25">
@@ -11265,7 +11270,7 @@
       <c r="V13" s="7"/>
       <c r="W13" s="7"/>
       <c r="X13" s="9" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="Y13" s="7"/>
     </row>
@@ -11298,7 +11303,7 @@
       <c r="V14" s="7"/>
       <c r="W14" s="7"/>
       <c r="X14" s="9" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="Y14" s="7"/>
     </row>
@@ -11331,7 +11336,7 @@
       <c r="V15" s="7"/>
       <c r="W15" s="7"/>
       <c r="X15" s="9" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="Y15" s="7"/>
     </row>
@@ -11364,7 +11369,7 @@
       <c r="V16" s="7"/>
       <c r="W16" s="7"/>
       <c r="X16" s="9" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="Y16" s="7"/>
     </row>
@@ -11397,7 +11402,7 @@
       <c r="V17" s="7"/>
       <c r="W17" s="7"/>
       <c r="X17" s="9" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="Y17" s="7"/>
     </row>
@@ -11471,7 +11476,7 @@
         <v>2020</v>
       </c>
       <c r="Y22" s="6" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="23" spans="1:25" x14ac:dyDescent="0.25">
@@ -11503,7 +11508,7 @@
       <c r="V23" s="7"/>
       <c r="W23" s="7"/>
       <c r="X23" s="9" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="Y23" s="7"/>
     </row>
@@ -11536,7 +11541,7 @@
       <c r="V24" s="7"/>
       <c r="W24" s="7"/>
       <c r="X24" s="9" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="Y24" s="7"/>
     </row>
@@ -11567,7 +11572,7 @@
       <c r="V25" s="7"/>
       <c r="W25" s="7"/>
       <c r="X25" s="9" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="Y25" s="7"/>
     </row>
@@ -11598,7 +11603,7 @@
       <c r="V26" s="7"/>
       <c r="W26" s="7"/>
       <c r="X26" s="9" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="Y26" s="7"/>
     </row>
@@ -11629,7 +11634,7 @@
       <c r="V27" s="7"/>
       <c r="W27" s="7"/>
       <c r="X27" s="9" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="Y27" s="7"/>
     </row>
@@ -11703,7 +11708,7 @@
         <v>2020</v>
       </c>
       <c r="Y32" s="6" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="33" spans="1:25" x14ac:dyDescent="0.25">
@@ -11735,7 +11740,7 @@
       <c r="V33" s="12"/>
       <c r="W33" s="12"/>
       <c r="X33" s="9" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="Y33" s="12"/>
     </row>
@@ -11768,7 +11773,7 @@
       <c r="V34" s="12"/>
       <c r="W34" s="12"/>
       <c r="X34" s="9" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="Y34" s="12"/>
     </row>
@@ -11801,7 +11806,7 @@
       <c r="V35" s="12"/>
       <c r="W35" s="12"/>
       <c r="X35" s="9" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="Y35" s="12"/>
     </row>
@@ -11834,7 +11839,7 @@
       <c r="V36" s="12"/>
       <c r="W36" s="12"/>
       <c r="X36" s="9" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="Y36" s="12"/>
     </row>
@@ -11867,13 +11872,13 @@
       <c r="V37" s="12"/>
       <c r="W37" s="12"/>
       <c r="X37" s="9" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="Y37" s="12"/>
     </row>
     <row r="41" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A41" s="4" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="42" spans="1:25" x14ac:dyDescent="0.25">
@@ -11941,7 +11946,7 @@
         <v>2020</v>
       </c>
       <c r="Y42" s="6" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="43" spans="1:25" x14ac:dyDescent="0.25">
@@ -11973,7 +11978,7 @@
       <c r="V43" s="12"/>
       <c r="W43" s="12"/>
       <c r="X43" s="9" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="Y43" s="12"/>
     </row>
@@ -12006,7 +12011,7 @@
       <c r="V44" s="12"/>
       <c r="W44" s="12"/>
       <c r="X44" s="9" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="Y44" s="12"/>
     </row>
@@ -12039,7 +12044,7 @@
       <c r="V45" s="12"/>
       <c r="W45" s="12"/>
       <c r="X45" s="9" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="Y45" s="12"/>
     </row>
@@ -12072,7 +12077,7 @@
       <c r="V46" s="12"/>
       <c r="W46" s="12"/>
       <c r="X46" s="9" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="Y46" s="12"/>
     </row>
@@ -12105,13 +12110,13 @@
       <c r="V47" s="12"/>
       <c r="W47" s="12"/>
       <c r="X47" s="9" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="Y47" s="12"/>
     </row>
     <row r="51" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A51" s="4" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="52" spans="1:25" x14ac:dyDescent="0.25">
@@ -12179,7 +12184,7 @@
         <v>2020</v>
       </c>
       <c r="Y52" s="6" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="53" spans="1:25" x14ac:dyDescent="0.25">
@@ -12211,7 +12216,7 @@
       <c r="V53" s="12"/>
       <c r="W53" s="12"/>
       <c r="X53" s="9" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="Y53" s="12"/>
     </row>
@@ -12244,7 +12249,7 @@
       <c r="V54" s="12"/>
       <c r="W54" s="12"/>
       <c r="X54" s="9" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="Y54" s="12"/>
     </row>
@@ -12275,7 +12280,7 @@
       <c r="V55" s="12"/>
       <c r="W55" s="12"/>
       <c r="X55" s="9" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="Y55" s="12">
         <v>0</v>
@@ -12308,7 +12313,7 @@
       <c r="V56" s="12"/>
       <c r="W56" s="12"/>
       <c r="X56" s="9" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="Y56" s="12">
         <v>0</v>
@@ -12341,7 +12346,7 @@
       <c r="V57" s="12"/>
       <c r="W57" s="12"/>
       <c r="X57" s="9" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="Y57" s="12">
         <v>0</v>
@@ -12349,7 +12354,7 @@
     </row>
     <row r="61" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A61" s="4" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="62" spans="1:25" x14ac:dyDescent="0.25">
@@ -12417,7 +12422,7 @@
         <v>2020</v>
       </c>
       <c r="Y62" s="6" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="63" spans="1:25" x14ac:dyDescent="0.25">
@@ -12449,7 +12454,7 @@
       <c r="V63" s="12"/>
       <c r="W63" s="12"/>
       <c r="X63" s="9" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="Y63" s="12"/>
     </row>
@@ -12482,7 +12487,7 @@
       <c r="V64" s="12"/>
       <c r="W64" s="12"/>
       <c r="X64" s="9" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="Y64" s="12"/>
     </row>
@@ -12515,7 +12520,7 @@
       <c r="V65" s="12"/>
       <c r="W65" s="12"/>
       <c r="X65" s="9" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="Y65" s="12"/>
     </row>
@@ -12544,7 +12549,7 @@
   <sheetData>
     <row r="1" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="2" spans="1:25" x14ac:dyDescent="0.25">
@@ -12612,7 +12617,7 @@
         <v>2020</v>
       </c>
       <c r="Y2" s="6" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="3" spans="1:25" x14ac:dyDescent="0.25">
@@ -12644,7 +12649,7 @@
       <c r="V3" s="7"/>
       <c r="W3" s="7"/>
       <c r="X3" s="9" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="Y3" s="7"/>
     </row>
@@ -12675,7 +12680,7 @@
       <c r="V4" s="7"/>
       <c r="W4" s="7"/>
       <c r="X4" s="9" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="Y4" s="7">
         <v>0</v>
@@ -12710,7 +12715,7 @@
       <c r="V5" s="7"/>
       <c r="W5" s="7"/>
       <c r="X5" s="9" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="Y5" s="7"/>
     </row>
@@ -12741,7 +12746,7 @@
       <c r="V6" s="7"/>
       <c r="W6" s="7"/>
       <c r="X6" s="9" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="Y6" s="7">
         <v>0</v>
@@ -12774,7 +12779,7 @@
       <c r="V7" s="7"/>
       <c r="W7" s="7"/>
       <c r="X7" s="9" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="Y7" s="7">
         <v>0</v>
@@ -12782,7 +12787,7 @@
     </row>
     <row r="11" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="12" spans="1:25" x14ac:dyDescent="0.25">
@@ -12850,7 +12855,7 @@
         <v>2020</v>
       </c>
       <c r="Y12" s="6" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="13" spans="1:25" x14ac:dyDescent="0.25">
@@ -12880,7 +12885,7 @@
       <c r="V13" s="12"/>
       <c r="W13" s="12"/>
       <c r="X13" s="9" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="Y13" s="12">
         <v>0.2</v>
@@ -12913,7 +12918,7 @@
       <c r="V14" s="12"/>
       <c r="W14" s="12"/>
       <c r="X14" s="9" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="Y14" s="12">
         <v>0</v>
@@ -12946,7 +12951,7 @@
       <c r="V15" s="12"/>
       <c r="W15" s="12"/>
       <c r="X15" s="9" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="Y15" s="12">
         <v>0.2</v>
@@ -12979,7 +12984,7 @@
       <c r="V16" s="12"/>
       <c r="W16" s="12"/>
       <c r="X16" s="9" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="Y16" s="12">
         <v>0</v>
@@ -13012,7 +13017,7 @@
       <c r="V17" s="12"/>
       <c r="W17" s="12"/>
       <c r="X17" s="9" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="Y17" s="12">
         <v>0</v>
@@ -13020,7 +13025,7 @@
     </row>
     <row r="21" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="22" spans="1:25" x14ac:dyDescent="0.25">
@@ -13088,7 +13093,7 @@
         <v>2020</v>
       </c>
       <c r="Y22" s="6" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="23" spans="1:25" x14ac:dyDescent="0.25">
@@ -13117,7 +13122,7 @@
       <c r="V23" s="7"/>
       <c r="W23" s="7"/>
       <c r="X23" s="9" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="Y23" s="7">
         <v>0</v>

</xml_diff>

<commit_message>
fixed issue with calling list elements
</commit_message>
<xml_diff>
--- a/server/src/static/sudanexample.xlsx
+++ b/server/src/static/sudanexample.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="20" windowWidth="21240" windowHeight="13300" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="20" windowWidth="21240" windowHeight="13300" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="1" r:id="rId1"/>
@@ -730,6 +730,321 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="543" uniqueCount="167">
   <si>
+    <t>Number (or percentage) of women on PMTCT (Option B/B+)</t>
+  </si>
+  <si>
+    <t>Birth rate (births per woman per year)</t>
+  </si>
+  <si>
+    <t>Percentage of HIV-positive women who breastfeed</t>
+  </si>
+  <si>
+    <t>Average number of acts with regular partners per person per year</t>
+  </si>
+  <si>
+    <t>Average number of acts with casual partners per person per year</t>
+  </si>
+  <si>
+    <t>Average number of acts with commercial partners per person per year</t>
+  </si>
+  <si>
+    <t>Percentage of people who used a condom at last act with regular partners</t>
+  </si>
+  <si>
+    <t>O P T I M A</t>
+  </si>
+  <si>
+    <t>Welcome to the Optima data entry spreadsheet. This is where all data for the model will be entered. At first glance the spreadsheet looks complicated and confusing. Unfortunately, it is. So please ask someone from the Optima development team if you need help, or use the default contact (info@optimamodel.com).</t>
+  </si>
+  <si>
+    <t>I. LAYOUT OF THE SPREADSHEET</t>
+  </si>
+  <si>
+    <t>Treatment failure rate (% per year)</t>
+  </si>
+  <si>
+    <t>First-line treatment</t>
+  </si>
+  <si>
+    <t>Second-line treatment</t>
+  </si>
+  <si>
+    <t>Death rate (% mortality per year)</t>
+  </si>
+  <si>
+    <t>CD4(350-500)</t>
+  </si>
+  <si>
+    <t>On treatment</t>
+  </si>
+  <si>
+    <t>Tuberculosis cofactor</t>
+  </si>
+  <si>
+    <t>Relative transmissibility</t>
+  </si>
+  <si>
+    <t>Condom use</t>
+  </si>
+  <si>
+    <t>Circumcision</t>
+  </si>
+  <si>
+    <t>Diagnosis behavior change</t>
+  </si>
+  <si>
+    <t>Ulcerative STI cofactor increase</t>
+  </si>
+  <si>
+    <t>Discharging STI cofactor increase</t>
+  </si>
+  <si>
+    <t>Clients of sex workers</t>
+  </si>
+  <si>
+    <t>MSM</t>
+  </si>
+  <si>
+    <t>Men who have sex with men</t>
+  </si>
+  <si>
+    <t>Males 15-49</t>
+  </si>
+  <si>
+    <t>Other males (15-49)</t>
+  </si>
+  <si>
+    <t>Females 15-49</t>
+  </si>
+  <si>
+    <t>Other females (15-49)</t>
+  </si>
+  <si>
+    <t>Programs</t>
+  </si>
+  <si>
+    <t>SBCC</t>
+  </si>
+  <si>
+    <t>General population prevention</t>
+  </si>
+  <si>
+    <t>FSW programs</t>
+  </si>
+  <si>
+    <t>Programs for female sex workers and clients</t>
+  </si>
+  <si>
+    <t>MSM programs</t>
+  </si>
+  <si>
+    <t>Programs for men who have sex with men</t>
+  </si>
+  <si>
+    <t>HTC</t>
+  </si>
+  <si>
+    <t>HIV testing and counseling</t>
+  </si>
+  <si>
+    <t>ART</t>
+  </si>
+  <si>
+    <t>* For each parameter (as in, row in the worksheet), there needs to be at least one data point entered. The only exception to this is the sheet "Optional indicators", which may be left blank. If data are not available for a particular indicator, enter an assumption in the "Assumption" column, with a comment explaining how that value was derived.</t>
+  </si>
+  <si>
+    <t>* Economic data only need to be entered if you are performing economic analyses.</t>
+  </si>
+  <si>
+    <t>If a parameter is left completely blank, it will be assumed to be zero.</t>
+  </si>
+  <si>
+    <t>IV. QUESTIONS</t>
+  </si>
+  <si>
+    <t>If you have any questions, please contact us on</t>
+  </si>
+  <si>
+    <t>info@optimamodel.com</t>
+  </si>
+  <si>
+    <t>Populations</t>
+  </si>
+  <si>
+    <t>Short name</t>
+  </si>
+  <si>
+    <t>Long name</t>
+  </si>
+  <si>
+    <t>Male</t>
+  </si>
+  <si>
+    <t>Female</t>
+  </si>
+  <si>
+    <t>Injects</t>
+  </si>
+  <si>
+    <t>Has sex with men</t>
+  </si>
+  <si>
+    <t>Has sex with women</t>
+  </si>
+  <si>
+    <t>Sex worker</t>
+  </si>
+  <si>
+    <t>Client</t>
+  </si>
+  <si>
+    <t>FSW</t>
+  </si>
+  <si>
+    <t>Female sex workers</t>
+  </si>
+  <si>
+    <t>FALSE</t>
+  </si>
+  <si>
+    <t>TRUE</t>
+  </si>
+  <si>
+    <t>Clients</t>
+  </si>
+  <si>
+    <t>Percentage of population tested for HIV in the last 12 months</t>
+  </si>
+  <si>
+    <t>Probability of a person with CD4 &lt;200 being tested per year</t>
+  </si>
+  <si>
+    <t>Average</t>
+  </si>
+  <si>
+    <t>Number of people on first-line treatment</t>
+  </si>
+  <si>
+    <t>Number of people on subsequent lines of treatment</t>
+  </si>
+  <si>
+    <t>Treatment eligibility criterion</t>
+  </si>
+  <si>
+    <t>Percentage of people covered by pre-exposure prophylaxis</t>
+  </si>
+  <si>
+    <t>Gross domestic product</t>
+  </si>
+  <si>
+    <t>Government revenue</t>
+  </si>
+  <si>
+    <t>Government expenditure</t>
+  </si>
+  <si>
+    <t>Total domestic and international health expenditure</t>
+  </si>
+  <si>
+    <t>General government health expenditure</t>
+  </si>
+  <si>
+    <t>Domestic HIV spending</t>
+  </si>
+  <si>
+    <t>Global Fund HIV commitments</t>
+  </si>
+  <si>
+    <t>PEPFAR HIV commitments</t>
+  </si>
+  <si>
+    <t>Other international HIV commitments</t>
+  </si>
+  <si>
+    <t>Private HIV spending</t>
+  </si>
+  <si>
+    <t>HIV-related health care costs (excluding treatment)</t>
+  </si>
+  <si>
+    <t>Social mitigation costs</t>
+  </si>
+  <si>
+    <t>Percentage of people who used a condom at last act with casual partners</t>
+  </si>
+  <si>
+    <t>Percentage of people who used a condom at last act with commercial partners</t>
+  </si>
+  <si>
+    <t>Percentage of males who have been circumcised</t>
+  </si>
+  <si>
+    <t>Average number of injections per person per year</t>
+  </si>
+  <si>
+    <t>Average percentage of people who receptively shared a needle/syringe at last injection</t>
+  </si>
+  <si>
+    <t>This spreadsheet is divided into 12 sheets. All sheets need to be completed, except where noted below.</t>
+  </si>
+  <si>
+    <t>II. HOW TO ENTER DATA</t>
+  </si>
+  <si>
+    <t>Do not enter anything except actual data, apart from the small number of instances which allows optional input of output from other models for comparison and verification! Optima will fit to actual data and will interpolate between data points, so only enter data in the years that they belong. In addition, please feel free to add notes (either as comments for a given cell or in the blank cells to the right of each row) about the source of the data.</t>
+  </si>
+  <si>
+    <t>III. WHAT CAN BE LEFT BLANK</t>
+  </si>
+  <si>
+    <t>It can be confusing what can and cannot be left blank, but here are a few general principles:</t>
+  </si>
+  <si>
+    <t>* Nothing on the "Populations and programs" sheet can be blank.</t>
+  </si>
+  <si>
+    <t>CD4(500) to CD4(350-500)</t>
+  </si>
+  <si>
+    <t>CD4(200-350)</t>
+  </si>
+  <si>
+    <t>CD4(50-200)</t>
+  </si>
+  <si>
+    <t>CD4(&lt;50)</t>
+  </si>
+  <si>
+    <t>Disease progression rate (% per year)</t>
+  </si>
+  <si>
+    <t>Acute to CD4(&gt;500)</t>
+  </si>
+  <si>
+    <t>CD4(350,500) to CD4(200-350)</t>
+  </si>
+  <si>
+    <t>CD4(200-350) to CD4(50-200)</t>
+  </si>
+  <si>
+    <t>CD4(50-200) to CD4(&lt;50)</t>
+  </si>
+  <si>
+    <t>Treatment recovery rate (% per year)</t>
+  </si>
+  <si>
+    <t>CD4(350-500) to CD4(&gt;500)</t>
+  </si>
+  <si>
+    <t>CD4(200-350) to CD4(350-500)</t>
+  </si>
+  <si>
+    <t>CD4(50-200) to CD4(200-350)</t>
+  </si>
+  <si>
+    <t>CD4(&lt;50) to CD4(50-200)</t>
+  </si>
+  <si>
     <t>Number of people who inject drugs who are on opiate substitution therapy</t>
   </si>
   <si>
@@ -916,321 +1231,6 @@
   </si>
   <si>
     <t>Purchasing power parity</t>
-  </si>
-  <si>
-    <t>Gross domestic product</t>
-  </si>
-  <si>
-    <t>Government revenue</t>
-  </si>
-  <si>
-    <t>Government expenditure</t>
-  </si>
-  <si>
-    <t>Total domestic and international health expenditure</t>
-  </si>
-  <si>
-    <t>General government health expenditure</t>
-  </si>
-  <si>
-    <t>Domestic HIV spending</t>
-  </si>
-  <si>
-    <t>Global Fund HIV commitments</t>
-  </si>
-  <si>
-    <t>PEPFAR HIV commitments</t>
-  </si>
-  <si>
-    <t>Other international HIV commitments</t>
-  </si>
-  <si>
-    <t>Private HIV spending</t>
-  </si>
-  <si>
-    <t>HIV-related health care costs (excluding treatment)</t>
-  </si>
-  <si>
-    <t>Social mitigation costs</t>
-  </si>
-  <si>
-    <t>Percentage of people who used a condom at last act with casual partners</t>
-  </si>
-  <si>
-    <t>Percentage of people who used a condom at last act with commercial partners</t>
-  </si>
-  <si>
-    <t>Percentage of males who have been circumcised</t>
-  </si>
-  <si>
-    <t>Average number of injections per person per year</t>
-  </si>
-  <si>
-    <t>Average percentage of people who receptively shared a needle/syringe at last injection</t>
-  </si>
-  <si>
-    <t>This spreadsheet is divided into 12 sheets. All sheets need to be completed, except where noted below.</t>
-  </si>
-  <si>
-    <t>II. HOW TO ENTER DATA</t>
-  </si>
-  <si>
-    <t>Do not enter anything except actual data, apart from the small number of instances which allows optional input of output from other models for comparison and verification! Optima will fit to actual data and will interpolate between data points, so only enter data in the years that they belong. In addition, please feel free to add notes (either as comments for a given cell or in the blank cells to the right of each row) about the source of the data.</t>
-  </si>
-  <si>
-    <t>III. WHAT CAN BE LEFT BLANK</t>
-  </si>
-  <si>
-    <t>It can be confusing what can and cannot be left blank, but here are a few general principles:</t>
-  </si>
-  <si>
-    <t>* Nothing on the "Populations and programs" sheet can be blank.</t>
-  </si>
-  <si>
-    <t>CD4(500) to CD4(350-500)</t>
-  </si>
-  <si>
-    <t>CD4(200-350)</t>
-  </si>
-  <si>
-    <t>CD4(50-200)</t>
-  </si>
-  <si>
-    <t>CD4(&lt;50)</t>
-  </si>
-  <si>
-    <t>Disease progression rate (% per year)</t>
-  </si>
-  <si>
-    <t>Acute to CD4(&gt;500)</t>
-  </si>
-  <si>
-    <t>CD4(350,500) to CD4(200-350)</t>
-  </si>
-  <si>
-    <t>CD4(200-350) to CD4(50-200)</t>
-  </si>
-  <si>
-    <t>CD4(50-200) to CD4(&lt;50)</t>
-  </si>
-  <si>
-    <t>Treatment recovery rate (% per year)</t>
-  </si>
-  <si>
-    <t>CD4(350-500) to CD4(&gt;500)</t>
-  </si>
-  <si>
-    <t>CD4(200-350) to CD4(350-500)</t>
-  </si>
-  <si>
-    <t>CD4(50-200) to CD4(200-350)</t>
-  </si>
-  <si>
-    <t>CD4(&lt;50) to CD4(50-200)</t>
-  </si>
-  <si>
-    <t>Treatment failure rate (% per year)</t>
-  </si>
-  <si>
-    <t>First-line treatment</t>
-  </si>
-  <si>
-    <t>Second-line treatment</t>
-  </si>
-  <si>
-    <t>Death rate (% mortality per year)</t>
-  </si>
-  <si>
-    <t>CD4(350-500)</t>
-  </si>
-  <si>
-    <t>On treatment</t>
-  </si>
-  <si>
-    <t>Tuberculosis cofactor</t>
-  </si>
-  <si>
-    <t>Relative transmissibility</t>
-  </si>
-  <si>
-    <t>Condom use</t>
-  </si>
-  <si>
-    <t>Circumcision</t>
-  </si>
-  <si>
-    <t>Diagnosis behavior change</t>
-  </si>
-  <si>
-    <t>Ulcerative STI cofactor increase</t>
-  </si>
-  <si>
-    <t>Discharging STI cofactor increase</t>
-  </si>
-  <si>
-    <t>Clients of sex workers</t>
-  </si>
-  <si>
-    <t>MSM</t>
-  </si>
-  <si>
-    <t>Men who have sex with men</t>
-  </si>
-  <si>
-    <t>Males 15-49</t>
-  </si>
-  <si>
-    <t>Other males (15-49)</t>
-  </si>
-  <si>
-    <t>Females 15-49</t>
-  </si>
-  <si>
-    <t>Other females (15-49)</t>
-  </si>
-  <si>
-    <t>Programs</t>
-  </si>
-  <si>
-    <t>SBCC</t>
-  </si>
-  <si>
-    <t>General population prevention</t>
-  </si>
-  <si>
-    <t>FSW programs</t>
-  </si>
-  <si>
-    <t>Programs for female sex workers and clients</t>
-  </si>
-  <si>
-    <t>MSM programs</t>
-  </si>
-  <si>
-    <t>Programs for men who have sex with men</t>
-  </si>
-  <si>
-    <t>HTC</t>
-  </si>
-  <si>
-    <t>HIV testing and counseling</t>
-  </si>
-  <si>
-    <t>ART</t>
-  </si>
-  <si>
-    <t>* For each parameter (as in, row in the worksheet), there needs to be at least one data point entered. The only exception to this is the sheet "Optional indicators", which may be left blank. If data are not available for a particular indicator, enter an assumption in the "Assumption" column, with a comment explaining how that value was derived.</t>
-  </si>
-  <si>
-    <t>* Economic data only need to be entered if you are performing economic analyses.</t>
-  </si>
-  <si>
-    <t>If a parameter is left completely blank, it will be assumed to be zero.</t>
-  </si>
-  <si>
-    <t>IV. QUESTIONS</t>
-  </si>
-  <si>
-    <t>If you have any questions, please contact us on</t>
-  </si>
-  <si>
-    <t>info@optimamodel.com</t>
-  </si>
-  <si>
-    <t>Populations</t>
-  </si>
-  <si>
-    <t>Short name</t>
-  </si>
-  <si>
-    <t>Long name</t>
-  </si>
-  <si>
-    <t>Male</t>
-  </si>
-  <si>
-    <t>Female</t>
-  </si>
-  <si>
-    <t>Injects</t>
-  </si>
-  <si>
-    <t>Has sex with men</t>
-  </si>
-  <si>
-    <t>Has sex with women</t>
-  </si>
-  <si>
-    <t>Sex worker</t>
-  </si>
-  <si>
-    <t>Client</t>
-  </si>
-  <si>
-    <t>FSW</t>
-  </si>
-  <si>
-    <t>Female sex workers</t>
-  </si>
-  <si>
-    <t>FALSE</t>
-  </si>
-  <si>
-    <t>TRUE</t>
-  </si>
-  <si>
-    <t>Clients</t>
-  </si>
-  <si>
-    <t>Percentage of population tested for HIV in the last 12 months</t>
-  </si>
-  <si>
-    <t>Probability of a person with CD4 &lt;200 being tested per year</t>
-  </si>
-  <si>
-    <t>Average</t>
-  </si>
-  <si>
-    <t>Number of people on first-line treatment</t>
-  </si>
-  <si>
-    <t>Number of people on subsequent lines of treatment</t>
-  </si>
-  <si>
-    <t>Treatment eligibility criterion</t>
-  </si>
-  <si>
-    <t>Percentage of people covered by pre-exposure prophylaxis</t>
-  </si>
-  <si>
-    <t>Number (or percentage) of women on PMTCT (Option B/B+)</t>
-  </si>
-  <si>
-    <t>Birth rate (births per woman per year)</t>
-  </si>
-  <si>
-    <t>Percentage of HIV-positive women who breastfeed</t>
-  </si>
-  <si>
-    <t>Average number of acts with regular partners per person per year</t>
-  </si>
-  <si>
-    <t>Average number of acts with casual partners per person per year</t>
-  </si>
-  <si>
-    <t>Average number of acts with commercial partners per person per year</t>
-  </si>
-  <si>
-    <t>Percentage of people who used a condom at last act with regular partners</t>
-  </si>
-  <si>
-    <t>O P T I M A</t>
-  </si>
-  <si>
-    <t>Welcome to the Optima data entry spreadsheet. This is where all data for the model will be entered. At first glance the spreadsheet looks complicated and confusing. Unfortunately, it is. So please ask someone from the Optima development team if you need help, or use the default contact (info@optimamodel.com).</t>
-  </si>
-  <si>
-    <t>I. LAYOUT OF THE SPREADSHEET</t>
   </si>
 </sst>
 </file>
@@ -1408,7 +1408,7 @@
     <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1487,6 +1487,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -1804,7 +1807,7 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" s="27" t="s">
-        <v>164</v>
+        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:1">
@@ -1818,7 +1821,7 @@
     </row>
     <row r="5" spans="1:1" ht="65" customHeight="1">
       <c r="A5" s="1" t="s">
-        <v>165</v>
+        <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:1">
@@ -1826,7 +1829,7 @@
     </row>
     <row r="7" spans="1:1">
       <c r="A7" s="2" t="s">
-        <v>166</v>
+        <v>9</v>
       </c>
     </row>
     <row r="8" spans="1:1">
@@ -1834,7 +1837,7 @@
     </row>
     <row r="9" spans="1:1">
       <c r="A9" s="1" t="s">
-        <v>79</v>
+        <v>85</v>
       </c>
     </row>
     <row r="10" spans="1:1">
@@ -1842,7 +1845,7 @@
     </row>
     <row r="11" spans="1:1">
       <c r="A11" s="2" t="s">
-        <v>80</v>
+        <v>86</v>
       </c>
     </row>
     <row r="12" spans="1:1">
@@ -1850,7 +1853,7 @@
     </row>
     <row r="13" spans="1:1" ht="80" customHeight="1">
       <c r="A13" s="1" t="s">
-        <v>81</v>
+        <v>87</v>
       </c>
     </row>
     <row r="14" spans="1:1">
@@ -1858,7 +1861,7 @@
     </row>
     <row r="15" spans="1:1">
       <c r="A15" s="2" t="s">
-        <v>82</v>
+        <v>88</v>
       </c>
     </row>
     <row r="16" spans="1:1">
@@ -1866,22 +1869,22 @@
     </row>
     <row r="17" spans="1:1">
       <c r="A17" s="1" t="s">
-        <v>83</v>
+        <v>89</v>
       </c>
     </row>
     <row r="18" spans="1:1">
       <c r="A18" s="1" t="s">
-        <v>84</v>
+        <v>90</v>
       </c>
     </row>
     <row r="19" spans="1:1" ht="57" customHeight="1">
       <c r="A19" s="1" t="s">
-        <v>129</v>
+        <v>40</v>
       </c>
     </row>
     <row r="20" spans="1:1">
       <c r="A20" s="1" t="s">
-        <v>130</v>
+        <v>41</v>
       </c>
     </row>
     <row r="21" spans="1:1">
@@ -1889,7 +1892,7 @@
     </row>
     <row r="22" spans="1:1">
       <c r="A22" s="1" t="s">
-        <v>131</v>
+        <v>42</v>
       </c>
     </row>
     <row r="23" spans="1:1">
@@ -1897,7 +1900,7 @@
     </row>
     <row r="24" spans="1:1">
       <c r="A24" s="2" t="s">
-        <v>132</v>
+        <v>43</v>
       </c>
     </row>
     <row r="25" spans="1:1">
@@ -1905,7 +1908,7 @@
     </row>
     <row r="26" spans="1:1">
       <c r="A26" s="1" t="s">
-        <v>133</v>
+        <v>44</v>
       </c>
     </row>
     <row r="27" spans="1:1">
@@ -1913,14 +1916,13 @@
     </row>
     <row r="28" spans="1:1">
       <c r="A28" s="3" t="s">
-        <v>134</v>
+        <v>45</v>
       </c>
     </row>
     <row r="29" spans="1:1">
       <c r="A29" s="1"/>
     </row>
   </sheetData>
-  <sheetCalcPr fullCalcOnLoad="1"/>
   <mergeCells count="1">
     <mergeCell ref="A1:A3"/>
   </mergeCells>
@@ -1953,7 +1955,7 @@
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" s="4" t="s">
-        <v>1</v>
+        <v>106</v>
       </c>
     </row>
     <row r="2" spans="1:7">
@@ -2047,7 +2049,7 @@
     </row>
     <row r="11" spans="1:7">
       <c r="A11" s="4" t="s">
-        <v>2</v>
+        <v>107</v>
       </c>
     </row>
     <row r="12" spans="1:7">
@@ -2141,7 +2143,7 @@
     </row>
     <row r="21" spans="1:7">
       <c r="A21" s="4" t="s">
-        <v>3</v>
+        <v>108</v>
       </c>
     </row>
     <row r="22" spans="1:7">
@@ -2225,7 +2227,7 @@
     </row>
     <row r="31" spans="1:7">
       <c r="A31" s="4" t="s">
-        <v>4</v>
+        <v>109</v>
       </c>
     </row>
     <row r="32" spans="1:7">
@@ -2310,7 +2312,6 @@
       <c r="G37" s="7"/>
     </row>
   </sheetData>
-  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
@@ -2337,7 +2338,7 @@
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" s="4" t="s">
-        <v>5</v>
+        <v>110</v>
       </c>
     </row>
     <row r="2" spans="1:7">
@@ -2419,7 +2420,7 @@
     </row>
     <row r="11" spans="1:7">
       <c r="A11" s="4" t="s">
-        <v>6</v>
+        <v>111</v>
       </c>
     </row>
     <row r="12" spans="1:7">
@@ -2504,7 +2505,6 @@
       <c r="G17" s="7"/>
     </row>
   </sheetData>
-  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
@@ -2529,23 +2529,23 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" s="4" t="s">
-        <v>7</v>
+        <v>112</v>
       </c>
     </row>
     <row r="2" spans="1:5">
       <c r="C2" s="6" t="s">
-        <v>34</v>
+        <v>139</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>35</v>
+        <v>140</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>33</v>
+        <v>138</v>
       </c>
     </row>
     <row r="3" spans="1:5">
       <c r="B3" s="5" t="s">
-        <v>8</v>
+        <v>113</v>
       </c>
       <c r="C3" s="8">
         <v>4.0000000000000002E-4</v>
@@ -2559,7 +2559,7 @@
     </row>
     <row r="4" spans="1:5">
       <c r="B4" s="5" t="s">
-        <v>9</v>
+        <v>114</v>
       </c>
       <c r="C4" s="8">
         <v>8.0000000000000004E-4</v>
@@ -2573,7 +2573,7 @@
     </row>
     <row r="5" spans="1:5">
       <c r="B5" s="5" t="s">
-        <v>10</v>
+        <v>115</v>
       </c>
       <c r="C5" s="8">
         <v>1.38E-2</v>
@@ -2587,7 +2587,7 @@
     </row>
     <row r="6" spans="1:5">
       <c r="B6" s="5" t="s">
-        <v>11</v>
+        <v>116</v>
       </c>
       <c r="C6" s="8">
         <v>1.1000000000000001E-3</v>
@@ -2601,7 +2601,7 @@
     </row>
     <row r="7" spans="1:5">
       <c r="B7" s="5" t="s">
-        <v>12</v>
+        <v>117</v>
       </c>
       <c r="C7" s="8">
         <v>8.0000000000000002E-3</v>
@@ -2615,7 +2615,7 @@
     </row>
     <row r="8" spans="1:5">
       <c r="B8" s="5" t="s">
-        <v>13</v>
+        <v>118</v>
       </c>
       <c r="C8" s="8">
         <v>0.36699999999999999</v>
@@ -2629,7 +2629,7 @@
     </row>
     <row r="9" spans="1:5">
       <c r="B9" s="5" t="s">
-        <v>14</v>
+        <v>119</v>
       </c>
       <c r="C9" s="8">
         <v>0.20499999999999999</v>
@@ -2643,23 +2643,23 @@
     </row>
     <row r="13" spans="1:5">
       <c r="A13" s="4" t="s">
-        <v>15</v>
+        <v>120</v>
       </c>
     </row>
     <row r="14" spans="1:5">
       <c r="C14" s="6" t="s">
-        <v>34</v>
+        <v>139</v>
       </c>
       <c r="D14" s="6" t="s">
-        <v>35</v>
+        <v>140</v>
       </c>
       <c r="E14" s="6" t="s">
-        <v>33</v>
+        <v>138</v>
       </c>
     </row>
     <row r="15" spans="1:5">
       <c r="B15" s="5" t="s">
-        <v>16</v>
+        <v>121</v>
       </c>
       <c r="C15" s="11">
         <v>26.03</v>
@@ -2673,7 +2673,7 @@
     </row>
     <row r="16" spans="1:5">
       <c r="B16" s="5" t="s">
-        <v>17</v>
+        <v>122</v>
       </c>
       <c r="C16" s="11">
         <v>1</v>
@@ -2687,7 +2687,7 @@
     </row>
     <row r="17" spans="1:5">
       <c r="B17" s="5" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="C17" s="11">
         <v>1</v>
@@ -2701,7 +2701,7 @@
     </row>
     <row r="18" spans="1:5">
       <c r="B18" s="5" t="s">
-        <v>86</v>
+        <v>92</v>
       </c>
       <c r="C18" s="11">
         <v>1</v>
@@ -2715,7 +2715,7 @@
     </row>
     <row r="19" spans="1:5">
       <c r="B19" s="5" t="s">
-        <v>87</v>
+        <v>93</v>
       </c>
       <c r="C19" s="11">
         <v>3.49</v>
@@ -2729,7 +2729,7 @@
     </row>
     <row r="20" spans="1:5">
       <c r="B20" s="5" t="s">
-        <v>88</v>
+        <v>94</v>
       </c>
       <c r="C20" s="11">
         <v>7.17</v>
@@ -2743,23 +2743,23 @@
     </row>
     <row r="24" spans="1:5">
       <c r="A24" s="4" t="s">
-        <v>89</v>
+        <v>95</v>
       </c>
     </row>
     <row r="25" spans="1:5">
       <c r="C25" s="6" t="s">
-        <v>34</v>
+        <v>139</v>
       </c>
       <c r="D25" s="6" t="s">
-        <v>35</v>
+        <v>140</v>
       </c>
       <c r="E25" s="6" t="s">
-        <v>33</v>
+        <v>138</v>
       </c>
     </row>
     <row r="26" spans="1:5">
       <c r="B26" s="5" t="s">
-        <v>90</v>
+        <v>96</v>
       </c>
       <c r="C26" s="12">
         <v>4.1399999999999997</v>
@@ -2773,7 +2773,7 @@
     </row>
     <row r="27" spans="1:5">
       <c r="B27" s="5" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="C27" s="12">
         <v>1.05</v>
@@ -2787,7 +2787,7 @@
     </row>
     <row r="28" spans="1:5">
       <c r="B28" s="5" t="s">
-        <v>91</v>
+        <v>97</v>
       </c>
       <c r="C28" s="12">
         <v>0.33</v>
@@ -2801,7 +2801,7 @@
     </row>
     <row r="29" spans="1:5">
       <c r="B29" s="5" t="s">
-        <v>92</v>
+        <v>98</v>
       </c>
       <c r="C29" s="12">
         <v>0.27</v>
@@ -2815,7 +2815,7 @@
     </row>
     <row r="30" spans="1:5">
       <c r="B30" s="5" t="s">
-        <v>93</v>
+        <v>99</v>
       </c>
       <c r="C30" s="12">
         <v>0.67</v>
@@ -2829,23 +2829,23 @@
     </row>
     <row r="34" spans="1:5">
       <c r="A34" s="4" t="s">
-        <v>94</v>
+        <v>100</v>
       </c>
     </row>
     <row r="35" spans="1:5">
       <c r="C35" s="6" t="s">
-        <v>34</v>
+        <v>139</v>
       </c>
       <c r="D35" s="6" t="s">
-        <v>35</v>
+        <v>140</v>
       </c>
       <c r="E35" s="6" t="s">
-        <v>33</v>
+        <v>138</v>
       </c>
     </row>
     <row r="36" spans="1:5">
       <c r="B36" s="5" t="s">
-        <v>95</v>
+        <v>101</v>
       </c>
       <c r="C36" s="12">
         <v>0.45</v>
@@ -2859,7 +2859,7 @@
     </row>
     <row r="37" spans="1:5">
       <c r="B37" s="5" t="s">
-        <v>96</v>
+        <v>102</v>
       </c>
       <c r="C37" s="12">
         <v>0.7</v>
@@ -2873,7 +2873,7 @@
     </row>
     <row r="38" spans="1:5">
       <c r="B38" s="5" t="s">
-        <v>97</v>
+        <v>103</v>
       </c>
       <c r="C38" s="12">
         <v>0.47</v>
@@ -2887,7 +2887,7 @@
     </row>
     <row r="39" spans="1:5">
       <c r="B39" s="5" t="s">
-        <v>98</v>
+        <v>104</v>
       </c>
       <c r="C39" s="12">
         <v>1.52</v>
@@ -2901,23 +2901,23 @@
     </row>
     <row r="43" spans="1:5">
       <c r="A43" s="4" t="s">
-        <v>99</v>
+        <v>10</v>
       </c>
     </row>
     <row r="44" spans="1:5">
       <c r="C44" s="6" t="s">
-        <v>34</v>
+        <v>139</v>
       </c>
       <c r="D44" s="6" t="s">
-        <v>35</v>
+        <v>140</v>
       </c>
       <c r="E44" s="6" t="s">
-        <v>33</v>
+        <v>138</v>
       </c>
     </row>
     <row r="45" spans="1:5">
       <c r="B45" s="5" t="s">
-        <v>100</v>
+        <v>11</v>
       </c>
       <c r="C45" s="12">
         <v>0.1</v>
@@ -2931,7 +2931,7 @@
     </row>
     <row r="46" spans="1:5">
       <c r="B46" s="5" t="s">
-        <v>101</v>
+        <v>12</v>
       </c>
       <c r="C46" s="12">
         <v>0.16</v>
@@ -2945,23 +2945,23 @@
     </row>
     <row r="50" spans="1:5">
       <c r="A50" s="4" t="s">
-        <v>102</v>
+        <v>13</v>
       </c>
     </row>
     <row r="51" spans="1:5">
       <c r="C51" s="6" t="s">
-        <v>34</v>
+        <v>139</v>
       </c>
       <c r="D51" s="6" t="s">
-        <v>35</v>
+        <v>140</v>
       </c>
       <c r="E51" s="6" t="s">
-        <v>33</v>
+        <v>138</v>
       </c>
     </row>
     <row r="52" spans="1:5">
       <c r="B52" s="5" t="s">
-        <v>16</v>
+        <v>121</v>
       </c>
       <c r="C52" s="8">
         <v>3.5999999999999999E-3</v>
@@ -2975,7 +2975,7 @@
     </row>
     <row r="53" spans="1:5">
       <c r="B53" s="5" t="s">
-        <v>17</v>
+        <v>122</v>
       </c>
       <c r="C53" s="8">
         <v>3.5999999999999999E-3</v>
@@ -2989,7 +2989,7 @@
     </row>
     <row r="54" spans="1:5">
       <c r="B54" s="5" t="s">
-        <v>103</v>
+        <v>14</v>
       </c>
       <c r="C54" s="8">
         <v>5.7999999999999996E-3</v>
@@ -3003,7 +3003,7 @@
     </row>
     <row r="55" spans="1:5">
       <c r="B55" s="5" t="s">
-        <v>86</v>
+        <v>92</v>
       </c>
       <c r="C55" s="8">
         <v>8.8000000000000005E-3</v>
@@ -3017,7 +3017,7 @@
     </row>
     <row r="56" spans="1:5">
       <c r="B56" s="5" t="s">
-        <v>87</v>
+        <v>93</v>
       </c>
       <c r="C56" s="8">
         <v>5.8999999999999997E-2</v>
@@ -3031,7 +3031,7 @@
     </row>
     <row r="57" spans="1:5">
       <c r="B57" s="5" t="s">
-        <v>88</v>
+        <v>94</v>
       </c>
       <c r="C57" s="8">
         <v>0.32300000000000001</v>
@@ -3045,7 +3045,7 @@
     </row>
     <row r="58" spans="1:5">
       <c r="B58" s="5" t="s">
-        <v>104</v>
+        <v>15</v>
       </c>
       <c r="C58" s="8">
         <v>0.23</v>
@@ -3059,7 +3059,7 @@
     </row>
     <row r="59" spans="1:5">
       <c r="B59" s="5" t="s">
-        <v>105</v>
+        <v>16</v>
       </c>
       <c r="C59" s="8">
         <v>2.17</v>
@@ -3073,23 +3073,23 @@
     </row>
     <row r="63" spans="1:5">
       <c r="A63" s="4" t="s">
-        <v>106</v>
+        <v>17</v>
       </c>
     </row>
     <row r="64" spans="1:5">
       <c r="C64" s="6" t="s">
-        <v>34</v>
+        <v>139</v>
       </c>
       <c r="D64" s="6" t="s">
-        <v>35</v>
+        <v>140</v>
       </c>
       <c r="E64" s="6" t="s">
-        <v>33</v>
+        <v>138</v>
       </c>
     </row>
     <row r="65" spans="1:5">
       <c r="B65" s="5" t="s">
-        <v>107</v>
+        <v>18</v>
       </c>
       <c r="C65" s="12">
         <v>0.05</v>
@@ -3103,7 +3103,7 @@
     </row>
     <row r="66" spans="1:5">
       <c r="B66" s="5" t="s">
-        <v>108</v>
+        <v>19</v>
       </c>
       <c r="C66" s="12">
         <v>0.42</v>
@@ -3117,7 +3117,7 @@
     </row>
     <row r="67" spans="1:5">
       <c r="B67" s="5" t="s">
-        <v>109</v>
+        <v>20</v>
       </c>
       <c r="C67" s="12">
         <v>1</v>
@@ -3131,7 +3131,7 @@
     </row>
     <row r="68" spans="1:5">
       <c r="B68" s="5" t="s">
-        <v>110</v>
+        <v>21</v>
       </c>
       <c r="C68" s="12">
         <v>2.65</v>
@@ -3145,7 +3145,7 @@
     </row>
     <row r="69" spans="1:5">
       <c r="B69" s="5" t="s">
-        <v>111</v>
+        <v>22</v>
       </c>
       <c r="C69" s="12">
         <v>1</v>
@@ -3159,7 +3159,7 @@
     </row>
     <row r="70" spans="1:5">
       <c r="B70" s="5" t="s">
-        <v>48</v>
+        <v>153</v>
       </c>
       <c r="C70" s="12">
         <v>0.46</v>
@@ -3173,7 +3173,7 @@
     </row>
     <row r="71" spans="1:5">
       <c r="B71" s="5" t="s">
-        <v>23</v>
+        <v>128</v>
       </c>
       <c r="C71" s="12">
         <v>0.1</v>
@@ -3187,7 +3187,7 @@
     </row>
     <row r="72" spans="1:5">
       <c r="B72" s="5" t="s">
-        <v>22</v>
+        <v>127</v>
       </c>
       <c r="C72" s="12">
         <v>0.3</v>
@@ -3201,7 +3201,7 @@
     </row>
     <row r="73" spans="1:5">
       <c r="B73" s="5" t="s">
-        <v>49</v>
+        <v>154</v>
       </c>
       <c r="C73" s="12">
         <v>0.27500000000000002</v>
@@ -3215,23 +3215,23 @@
     </row>
     <row r="77" spans="1:5">
       <c r="A77" s="4" t="s">
-        <v>50</v>
+        <v>155</v>
       </c>
     </row>
     <row r="78" spans="1:5">
       <c r="C78" s="6" t="s">
-        <v>34</v>
+        <v>139</v>
       </c>
       <c r="D78" s="6" t="s">
-        <v>35</v>
+        <v>140</v>
       </c>
       <c r="E78" s="6" t="s">
-        <v>33</v>
+        <v>138</v>
       </c>
     </row>
     <row r="79" spans="1:5">
       <c r="B79" s="5" t="s">
-        <v>51</v>
+        <v>156</v>
       </c>
       <c r="C79" s="11">
         <v>0.14599999999999999</v>
@@ -3245,7 +3245,7 @@
     </row>
     <row r="80" spans="1:5">
       <c r="B80" s="5" t="s">
-        <v>52</v>
+        <v>157</v>
       </c>
       <c r="C80" s="11">
         <v>8.0000000000000002E-3</v>
@@ -3259,7 +3259,7 @@
     </row>
     <row r="81" spans="2:5">
       <c r="B81" s="5" t="s">
-        <v>53</v>
+        <v>158</v>
       </c>
       <c r="C81" s="11">
         <v>0.02</v>
@@ -3273,7 +3273,7 @@
     </row>
     <row r="82" spans="2:5">
       <c r="B82" s="5" t="s">
-        <v>54</v>
+        <v>159</v>
       </c>
       <c r="C82" s="11">
         <v>7.0000000000000007E-2</v>
@@ -3287,7 +3287,7 @@
     </row>
     <row r="83" spans="2:5">
       <c r="B83" s="5" t="s">
-        <v>55</v>
+        <v>160</v>
       </c>
       <c r="C83" s="11">
         <v>0.26500000000000001</v>
@@ -3301,7 +3301,7 @@
     </row>
     <row r="84" spans="2:5">
       <c r="B84" s="5" t="s">
-        <v>56</v>
+        <v>161</v>
       </c>
       <c r="C84" s="11">
         <v>0.54700000000000004</v>
@@ -3315,7 +3315,7 @@
     </row>
     <row r="85" spans="2:5">
       <c r="B85" s="5" t="s">
-        <v>57</v>
+        <v>162</v>
       </c>
       <c r="C85" s="11">
         <v>5.2999999999999999E-2</v>
@@ -3328,7 +3328,6 @@
       </c>
     </row>
   </sheetData>
-  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
@@ -3352,10 +3351,10 @@
   <sheetData>
     <row r="1" spans="1:27">
       <c r="A1" s="4" t="s">
-        <v>58</v>
+        <v>163</v>
       </c>
       <c r="Y1" s="6" t="s">
-        <v>59</v>
+        <v>164</v>
       </c>
     </row>
     <row r="2" spans="1:27">
@@ -3423,18 +3422,18 @@
         <v>2020</v>
       </c>
       <c r="Y2" s="6" t="s">
-        <v>34</v>
+        <v>139</v>
       </c>
       <c r="Z2" s="6" t="s">
-        <v>35</v>
+        <v>140</v>
       </c>
       <c r="AA2" s="6" t="s">
-        <v>33</v>
+        <v>138</v>
       </c>
     </row>
     <row r="3" spans="1:27">
       <c r="B3" s="6" t="s">
-        <v>38</v>
+        <v>143</v>
       </c>
       <c r="C3" s="22">
         <v>41.670326870927902</v>
@@ -3486,7 +3485,7 @@
       <c r="V3" s="10"/>
       <c r="W3" s="10"/>
       <c r="X3" s="9" t="s">
-        <v>60</v>
+        <v>165</v>
       </c>
       <c r="Y3" s="12">
         <v>0.2</v>
@@ -3500,7 +3499,7 @@
     </row>
     <row r="7" spans="1:27">
       <c r="A7" s="4" t="s">
-        <v>61</v>
+        <v>166</v>
       </c>
     </row>
     <row r="8" spans="1:27">
@@ -3568,18 +3567,18 @@
         <v>2020</v>
       </c>
       <c r="Y8" s="6" t="s">
-        <v>34</v>
+        <v>139</v>
       </c>
       <c r="Z8" s="6" t="s">
-        <v>35</v>
+        <v>140</v>
       </c>
       <c r="AA8" s="6" t="s">
-        <v>33</v>
+        <v>138</v>
       </c>
     </row>
     <row r="9" spans="1:27">
       <c r="B9" s="6" t="s">
-        <v>38</v>
+        <v>143</v>
       </c>
       <c r="C9" s="23">
         <v>0.482758166845627</v>
@@ -3631,7 +3630,7 @@
       <c r="V9" s="10"/>
       <c r="W9" s="10"/>
       <c r="X9" s="9" t="s">
-        <v>60</v>
+        <v>165</v>
       </c>
       <c r="Y9" s="12">
         <v>0.4</v>
@@ -3645,7 +3644,7 @@
     </row>
     <row r="13" spans="1:27">
       <c r="A13" s="4" t="s">
-        <v>62</v>
+        <v>68</v>
       </c>
     </row>
     <row r="14" spans="1:27">
@@ -3713,18 +3712,18 @@
         <v>2020</v>
       </c>
       <c r="Y14" s="6" t="s">
-        <v>34</v>
+        <v>139</v>
       </c>
       <c r="Z14" s="6" t="s">
-        <v>35</v>
+        <v>140</v>
       </c>
       <c r="AA14" s="6" t="s">
-        <v>33</v>
+        <v>138</v>
       </c>
     </row>
     <row r="15" spans="1:27">
       <c r="B15" s="6" t="s">
-        <v>38</v>
+        <v>143</v>
       </c>
       <c r="C15" s="13">
         <v>12257299147.293604</v>
@@ -3776,7 +3775,7 @@
       <c r="V15" s="10"/>
       <c r="W15" s="10"/>
       <c r="X15" s="9" t="s">
-        <v>60</v>
+        <v>165</v>
       </c>
       <c r="Y15" s="12">
         <v>0.05</v>
@@ -3790,7 +3789,7 @@
     </row>
     <row r="19" spans="1:27">
       <c r="A19" s="4" t="s">
-        <v>63</v>
+        <v>69</v>
       </c>
     </row>
     <row r="20" spans="1:27">
@@ -3858,18 +3857,18 @@
         <v>2020</v>
       </c>
       <c r="Y20" s="6" t="s">
-        <v>34</v>
+        <v>139</v>
       </c>
       <c r="Z20" s="6" t="s">
-        <v>35</v>
+        <v>140</v>
       </c>
       <c r="AA20" s="6" t="s">
-        <v>33</v>
+        <v>138</v>
       </c>
     </row>
     <row r="21" spans="1:27">
       <c r="B21" s="6" t="s">
-        <v>38</v>
+        <v>143</v>
       </c>
       <c r="C21" s="10"/>
       <c r="D21" s="10"/>
@@ -3893,7 +3892,7 @@
       <c r="V21" s="10"/>
       <c r="W21" s="10"/>
       <c r="X21" s="9" t="s">
-        <v>60</v>
+        <v>165</v>
       </c>
       <c r="Y21" s="10"/>
       <c r="Z21" s="10"/>
@@ -3901,7 +3900,7 @@
     </row>
     <row r="25" spans="1:27">
       <c r="A25" s="4" t="s">
-        <v>64</v>
+        <v>70</v>
       </c>
     </row>
     <row r="26" spans="1:27">
@@ -3969,18 +3968,18 @@
         <v>2020</v>
       </c>
       <c r="Y26" s="6" t="s">
-        <v>34</v>
+        <v>139</v>
       </c>
       <c r="Z26" s="6" t="s">
-        <v>35</v>
+        <v>140</v>
       </c>
       <c r="AA26" s="6" t="s">
-        <v>33</v>
+        <v>138</v>
       </c>
     </row>
     <row r="27" spans="1:27">
       <c r="B27" s="6" t="s">
-        <v>38</v>
+        <v>143</v>
       </c>
       <c r="C27" s="10"/>
       <c r="D27" s="10"/>
@@ -4004,7 +4003,7 @@
       <c r="V27" s="10"/>
       <c r="W27" s="10"/>
       <c r="X27" s="9" t="s">
-        <v>60</v>
+        <v>165</v>
       </c>
       <c r="Y27" s="10"/>
       <c r="Z27" s="10"/>
@@ -4012,7 +4011,7 @@
     </row>
     <row r="31" spans="1:27">
       <c r="A31" s="4" t="s">
-        <v>65</v>
+        <v>71</v>
       </c>
     </row>
     <row r="32" spans="1:27">
@@ -4080,18 +4079,18 @@
         <v>2020</v>
       </c>
       <c r="Y32" s="6" t="s">
-        <v>34</v>
+        <v>139</v>
       </c>
       <c r="Z32" s="6" t="s">
-        <v>35</v>
+        <v>140</v>
       </c>
       <c r="AA32" s="6" t="s">
-        <v>33</v>
+        <v>138</v>
       </c>
     </row>
     <row r="33" spans="1:27">
       <c r="B33" s="6" t="s">
-        <v>38</v>
+        <v>143</v>
       </c>
       <c r="C33" s="10"/>
       <c r="D33" s="10"/>
@@ -4115,7 +4114,7 @@
       <c r="V33" s="10"/>
       <c r="W33" s="10"/>
       <c r="X33" s="9" t="s">
-        <v>60</v>
+        <v>165</v>
       </c>
       <c r="Y33" s="10"/>
       <c r="Z33" s="10"/>
@@ -4123,7 +4122,7 @@
     </row>
     <row r="37" spans="1:27">
       <c r="A37" s="4" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
     </row>
     <row r="38" spans="1:27">
@@ -4191,18 +4190,18 @@
         <v>2020</v>
       </c>
       <c r="Y38" s="6" t="s">
-        <v>34</v>
+        <v>139</v>
       </c>
       <c r="Z38" s="6" t="s">
-        <v>35</v>
+        <v>140</v>
       </c>
       <c r="AA38" s="6" t="s">
-        <v>33</v>
+        <v>138</v>
       </c>
     </row>
     <row r="39" spans="1:27">
       <c r="B39" s="6" t="s">
-        <v>38</v>
+        <v>143</v>
       </c>
       <c r="C39" s="10"/>
       <c r="D39" s="10"/>
@@ -4226,7 +4225,7 @@
       <c r="V39" s="10"/>
       <c r="W39" s="10"/>
       <c r="X39" s="9" t="s">
-        <v>60</v>
+        <v>165</v>
       </c>
       <c r="Y39" s="10"/>
       <c r="Z39" s="10"/>
@@ -4234,7 +4233,7 @@
     </row>
     <row r="43" spans="1:27">
       <c r="A43" s="4" t="s">
-        <v>67</v>
+        <v>73</v>
       </c>
     </row>
     <row r="44" spans="1:27">
@@ -4302,18 +4301,18 @@
         <v>2020</v>
       </c>
       <c r="Y44" s="6" t="s">
-        <v>34</v>
+        <v>139</v>
       </c>
       <c r="Z44" s="6" t="s">
-        <v>35</v>
+        <v>140</v>
       </c>
       <c r="AA44" s="6" t="s">
-        <v>33</v>
+        <v>138</v>
       </c>
     </row>
     <row r="45" spans="1:27">
       <c r="B45" s="6" t="s">
-        <v>38</v>
+        <v>143</v>
       </c>
       <c r="C45" s="10"/>
       <c r="D45" s="10"/>
@@ -4337,7 +4336,7 @@
       <c r="V45" s="10"/>
       <c r="W45" s="10"/>
       <c r="X45" s="9" t="s">
-        <v>60</v>
+        <v>165</v>
       </c>
       <c r="Y45" s="10"/>
       <c r="Z45" s="10"/>
@@ -4345,7 +4344,7 @@
     </row>
     <row r="49" spans="1:27">
       <c r="A49" s="4" t="s">
-        <v>68</v>
+        <v>74</v>
       </c>
     </row>
     <row r="50" spans="1:27">
@@ -4413,18 +4412,18 @@
         <v>2020</v>
       </c>
       <c r="Y50" s="6" t="s">
-        <v>34</v>
+        <v>139</v>
       </c>
       <c r="Z50" s="6" t="s">
-        <v>35</v>
+        <v>140</v>
       </c>
       <c r="AA50" s="6" t="s">
-        <v>33</v>
+        <v>138</v>
       </c>
     </row>
     <row r="51" spans="1:27">
       <c r="B51" s="6" t="s">
-        <v>38</v>
+        <v>143</v>
       </c>
       <c r="C51" s="10"/>
       <c r="D51" s="10"/>
@@ -4448,7 +4447,7 @@
       <c r="V51" s="10"/>
       <c r="W51" s="10"/>
       <c r="X51" s="9" t="s">
-        <v>60</v>
+        <v>165</v>
       </c>
       <c r="Y51" s="10"/>
       <c r="Z51" s="10"/>
@@ -4456,7 +4455,7 @@
     </row>
     <row r="55" spans="1:27">
       <c r="A55" s="4" t="s">
-        <v>69</v>
+        <v>75</v>
       </c>
     </row>
     <row r="56" spans="1:27">
@@ -4524,18 +4523,18 @@
         <v>2020</v>
       </c>
       <c r="Y56" s="6" t="s">
-        <v>34</v>
+        <v>139</v>
       </c>
       <c r="Z56" s="6" t="s">
-        <v>35</v>
+        <v>140</v>
       </c>
       <c r="AA56" s="6" t="s">
-        <v>33</v>
+        <v>138</v>
       </c>
     </row>
     <row r="57" spans="1:27">
       <c r="B57" s="6" t="s">
-        <v>38</v>
+        <v>143</v>
       </c>
       <c r="C57" s="10"/>
       <c r="D57" s="10"/>
@@ -4559,7 +4558,7 @@
       <c r="V57" s="10"/>
       <c r="W57" s="10"/>
       <c r="X57" s="9" t="s">
-        <v>60</v>
+        <v>165</v>
       </c>
       <c r="Y57" s="10"/>
       <c r="Z57" s="10"/>
@@ -4567,7 +4566,7 @@
     </row>
     <row r="61" spans="1:27">
       <c r="A61" s="4" t="s">
-        <v>70</v>
+        <v>76</v>
       </c>
     </row>
     <row r="62" spans="1:27">
@@ -4635,18 +4634,18 @@
         <v>2020</v>
       </c>
       <c r="Y62" s="6" t="s">
-        <v>34</v>
+        <v>139</v>
       </c>
       <c r="Z62" s="6" t="s">
-        <v>35</v>
+        <v>140</v>
       </c>
       <c r="AA62" s="6" t="s">
-        <v>33</v>
+        <v>138</v>
       </c>
     </row>
     <row r="63" spans="1:27">
       <c r="B63" s="6" t="s">
-        <v>38</v>
+        <v>143</v>
       </c>
       <c r="C63" s="10"/>
       <c r="D63" s="10"/>
@@ -4670,7 +4669,7 @@
       <c r="V63" s="10"/>
       <c r="W63" s="10"/>
       <c r="X63" s="9" t="s">
-        <v>60</v>
+        <v>165</v>
       </c>
       <c r="Y63" s="10"/>
       <c r="Z63" s="10"/>
@@ -4678,7 +4677,7 @@
     </row>
     <row r="67" spans="1:27">
       <c r="A67" s="4" t="s">
-        <v>71</v>
+        <v>77</v>
       </c>
     </row>
     <row r="68" spans="1:27">
@@ -4746,18 +4745,18 @@
         <v>2020</v>
       </c>
       <c r="Y68" s="6" t="s">
-        <v>34</v>
+        <v>139</v>
       </c>
       <c r="Z68" s="6" t="s">
-        <v>35</v>
+        <v>140</v>
       </c>
       <c r="AA68" s="6" t="s">
-        <v>33</v>
+        <v>138</v>
       </c>
     </row>
     <row r="69" spans="1:27">
       <c r="B69" s="6" t="s">
-        <v>38</v>
+        <v>143</v>
       </c>
       <c r="C69" s="10"/>
       <c r="D69" s="10"/>
@@ -4781,7 +4780,7 @@
       <c r="V69" s="10"/>
       <c r="W69" s="10"/>
       <c r="X69" s="9" t="s">
-        <v>60</v>
+        <v>165</v>
       </c>
       <c r="Y69" s="10"/>
       <c r="Z69" s="10"/>
@@ -4789,7 +4788,7 @@
     </row>
     <row r="73" spans="1:27">
       <c r="A73" s="4" t="s">
-        <v>72</v>
+        <v>78</v>
       </c>
     </row>
     <row r="74" spans="1:27">
@@ -4857,18 +4856,18 @@
         <v>2020</v>
       </c>
       <c r="Y74" s="6" t="s">
-        <v>34</v>
+        <v>139</v>
       </c>
       <c r="Z74" s="6" t="s">
-        <v>35</v>
+        <v>140</v>
       </c>
       <c r="AA74" s="6" t="s">
-        <v>33</v>
+        <v>138</v>
       </c>
     </row>
     <row r="75" spans="1:27">
       <c r="B75" s="6" t="s">
-        <v>16</v>
+        <v>121</v>
       </c>
       <c r="C75" s="11"/>
       <c r="D75" s="11"/>
@@ -4894,7 +4893,7 @@
       <c r="V75" s="11"/>
       <c r="W75" s="11"/>
       <c r="X75" s="9" t="s">
-        <v>60</v>
+        <v>165</v>
       </c>
       <c r="Y75" s="24">
         <v>0.03</v>
@@ -4908,7 +4907,7 @@
     </row>
     <row r="76" spans="1:27">
       <c r="B76" s="6" t="s">
-        <v>17</v>
+        <v>122</v>
       </c>
       <c r="C76" s="11"/>
       <c r="D76" s="11"/>
@@ -4934,7 +4933,7 @@
       <c r="V76" s="11"/>
       <c r="W76" s="11"/>
       <c r="X76" s="9" t="s">
-        <v>60</v>
+        <v>165</v>
       </c>
       <c r="Y76" s="24">
         <v>0.03</v>
@@ -4948,7 +4947,7 @@
     </row>
     <row r="77" spans="1:27">
       <c r="B77" s="6" t="s">
-        <v>103</v>
+        <v>14</v>
       </c>
       <c r="C77" s="11"/>
       <c r="D77" s="11"/>
@@ -4974,7 +4973,7 @@
       <c r="V77" s="11"/>
       <c r="W77" s="11"/>
       <c r="X77" s="9" t="s">
-        <v>60</v>
+        <v>165</v>
       </c>
       <c r="Y77" s="24">
         <v>0.03</v>
@@ -4988,7 +4987,7 @@
     </row>
     <row r="78" spans="1:27">
       <c r="B78" s="6" t="s">
-        <v>86</v>
+        <v>92</v>
       </c>
       <c r="C78" s="11"/>
       <c r="D78" s="11"/>
@@ -5014,7 +5013,7 @@
       <c r="V78" s="11"/>
       <c r="W78" s="11"/>
       <c r="X78" s="9" t="s">
-        <v>60</v>
+        <v>165</v>
       </c>
       <c r="Y78" s="24">
         <v>0.03</v>
@@ -5028,7 +5027,7 @@
     </row>
     <row r="79" spans="1:27">
       <c r="B79" s="6" t="s">
-        <v>87</v>
+        <v>93</v>
       </c>
       <c r="C79" s="11"/>
       <c r="D79" s="11"/>
@@ -5054,7 +5053,7 @@
       <c r="V79" s="11"/>
       <c r="W79" s="11"/>
       <c r="X79" s="9" t="s">
-        <v>60</v>
+        <v>165</v>
       </c>
       <c r="Y79" s="24">
         <v>0.03</v>
@@ -5068,7 +5067,7 @@
     </row>
     <row r="80" spans="1:27">
       <c r="B80" s="6" t="s">
-        <v>88</v>
+        <v>94</v>
       </c>
       <c r="C80" s="11"/>
       <c r="D80" s="11"/>
@@ -5094,7 +5093,7 @@
       <c r="V80" s="11"/>
       <c r="W80" s="11"/>
       <c r="X80" s="9" t="s">
-        <v>60</v>
+        <v>165</v>
       </c>
       <c r="Y80" s="24">
         <v>0.03</v>
@@ -5117,7 +5116,7 @@
     </row>
     <row r="84" spans="1:27">
       <c r="A84" s="4" t="s">
-        <v>73</v>
+        <v>79</v>
       </c>
       <c r="Y84" s="25"/>
     </row>
@@ -5186,18 +5185,18 @@
         <v>2020</v>
       </c>
       <c r="Y85" s="26" t="s">
-        <v>34</v>
+        <v>139</v>
       </c>
       <c r="Z85" s="26" t="s">
-        <v>35</v>
+        <v>140</v>
       </c>
       <c r="AA85" s="26" t="s">
-        <v>33</v>
+        <v>138</v>
       </c>
     </row>
     <row r="86" spans="1:27">
       <c r="B86" s="6" t="s">
-        <v>16</v>
+        <v>121</v>
       </c>
       <c r="C86" s="11"/>
       <c r="D86" s="11"/>
@@ -5223,7 +5222,7 @@
       <c r="V86" s="11"/>
       <c r="W86" s="11"/>
       <c r="X86" s="9" t="s">
-        <v>60</v>
+        <v>165</v>
       </c>
       <c r="Y86" s="24">
         <v>0.03</v>
@@ -5237,7 +5236,7 @@
     </row>
     <row r="87" spans="1:27">
       <c r="B87" s="6" t="s">
-        <v>17</v>
+        <v>122</v>
       </c>
       <c r="C87" s="11"/>
       <c r="D87" s="11"/>
@@ -5263,7 +5262,7 @@
       <c r="V87" s="11"/>
       <c r="W87" s="11"/>
       <c r="X87" s="9" t="s">
-        <v>60</v>
+        <v>165</v>
       </c>
       <c r="Y87" s="24">
         <v>0.03</v>
@@ -5277,7 +5276,7 @@
     </row>
     <row r="88" spans="1:27">
       <c r="B88" s="6" t="s">
-        <v>103</v>
+        <v>14</v>
       </c>
       <c r="C88" s="11"/>
       <c r="D88" s="11"/>
@@ -5303,7 +5302,7 @@
       <c r="V88" s="11"/>
       <c r="W88" s="11"/>
       <c r="X88" s="9" t="s">
-        <v>60</v>
+        <v>165</v>
       </c>
       <c r="Y88" s="24">
         <v>0.03</v>
@@ -5317,7 +5316,7 @@
     </row>
     <row r="89" spans="1:27">
       <c r="B89" s="6" t="s">
-        <v>86</v>
+        <v>92</v>
       </c>
       <c r="C89" s="11"/>
       <c r="D89" s="11"/>
@@ -5343,7 +5342,7 @@
       <c r="V89" s="11"/>
       <c r="W89" s="11"/>
       <c r="X89" s="9" t="s">
-        <v>60</v>
+        <v>165</v>
       </c>
       <c r="Y89" s="24">
         <v>0.03</v>
@@ -5357,7 +5356,7 @@
     </row>
     <row r="90" spans="1:27">
       <c r="B90" s="6" t="s">
-        <v>87</v>
+        <v>93</v>
       </c>
       <c r="C90" s="11"/>
       <c r="D90" s="11"/>
@@ -5383,7 +5382,7 @@
       <c r="V90" s="11"/>
       <c r="W90" s="11"/>
       <c r="X90" s="9" t="s">
-        <v>60</v>
+        <v>165</v>
       </c>
       <c r="Y90" s="24">
         <v>0.03</v>
@@ -5397,7 +5396,7 @@
     </row>
     <row r="91" spans="1:27">
       <c r="B91" s="6" t="s">
-        <v>88</v>
+        <v>94</v>
       </c>
       <c r="C91" s="11"/>
       <c r="D91" s="11"/>
@@ -5423,7 +5422,7 @@
       <c r="V91" s="11"/>
       <c r="W91" s="11"/>
       <c r="X91" s="9" t="s">
-        <v>60</v>
+        <v>165</v>
       </c>
       <c r="Y91" s="24">
         <v>0.03</v>
@@ -5436,7 +5435,6 @@
       </c>
     </row>
   </sheetData>
-  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
@@ -5452,7 +5450,7 @@
   <sheetPr published="0" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:K21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
@@ -5467,36 +5465,36 @@
   <sheetData>
     <row r="1" spans="1:11">
       <c r="A1" s="4" t="s">
-        <v>135</v>
+        <v>46</v>
       </c>
     </row>
     <row r="2" spans="1:11">
       <c r="C2" s="5" t="s">
-        <v>136</v>
+        <v>47</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>137</v>
+        <v>48</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>138</v>
+        <v>49</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>139</v>
+        <v>50</v>
       </c>
       <c r="G2" s="5" t="s">
-        <v>140</v>
+        <v>51</v>
       </c>
       <c r="H2" s="5" t="s">
-        <v>141</v>
+        <v>52</v>
       </c>
       <c r="I2" s="5" t="s">
-        <v>142</v>
+        <v>53</v>
       </c>
       <c r="J2" s="5" t="s">
-        <v>143</v>
+        <v>54</v>
       </c>
       <c r="K2" s="5" t="s">
-        <v>144</v>
+        <v>55</v>
       </c>
     </row>
     <row r="3" spans="1:11">
@@ -5504,31 +5502,31 @@
         <v>1</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>145</v>
+        <v>56</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>146</v>
+        <v>57</v>
       </c>
       <c r="E3" s="7" t="s">
-        <v>147</v>
+        <v>58</v>
       </c>
       <c r="F3" s="7" t="s">
-        <v>148</v>
+        <v>59</v>
       </c>
       <c r="G3" s="7" t="s">
-        <v>148</v>
+        <v>59</v>
       </c>
       <c r="H3" s="7" t="s">
-        <v>148</v>
+        <v>59</v>
       </c>
       <c r="I3" s="7" t="s">
-        <v>147</v>
+        <v>58</v>
       </c>
       <c r="J3" s="7" t="s">
-        <v>148</v>
+        <v>59</v>
       </c>
       <c r="K3" s="7" t="s">
-        <v>147</v>
+        <v>58</v>
       </c>
     </row>
     <row r="4" spans="1:11">
@@ -5536,31 +5534,31 @@
         <v>2</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>149</v>
+        <v>60</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>112</v>
+        <v>23</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>148</v>
+        <v>59</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>147</v>
+        <v>58</v>
       </c>
       <c r="G4" s="7" t="s">
-        <v>147</v>
+        <v>58</v>
       </c>
       <c r="H4" s="7" t="s">
-        <v>147</v>
+        <v>58</v>
       </c>
       <c r="I4" s="7" t="s">
-        <v>148</v>
+        <v>59</v>
       </c>
       <c r="J4" s="7" t="s">
-        <v>147</v>
+        <v>58</v>
       </c>
       <c r="K4" s="7" t="s">
-        <v>148</v>
+        <v>59</v>
       </c>
     </row>
     <row r="5" spans="1:11">
@@ -5568,31 +5566,31 @@
         <v>3</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>113</v>
+        <v>24</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>114</v>
+        <v>25</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>148</v>
+        <v>59</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>147</v>
+        <v>58</v>
       </c>
       <c r="G5" s="7" t="s">
-        <v>148</v>
+        <v>59</v>
       </c>
       <c r="H5" s="7" t="s">
-        <v>148</v>
+        <v>59</v>
       </c>
       <c r="I5" s="7" t="s">
-        <v>148</v>
+        <v>59</v>
       </c>
       <c r="J5" s="7" t="s">
-        <v>147</v>
+        <v>58</v>
       </c>
       <c r="K5" s="7" t="s">
-        <v>147</v>
+        <v>58</v>
       </c>
     </row>
     <row r="6" spans="1:11">
@@ -5600,31 +5598,31 @@
         <v>4</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>115</v>
+        <v>26</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>116</v>
+        <v>27</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>148</v>
+        <v>59</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>147</v>
+        <v>58</v>
       </c>
       <c r="G6" s="7" t="s">
-        <v>147</v>
+        <v>58</v>
       </c>
       <c r="H6" s="7" t="s">
-        <v>147</v>
+        <v>58</v>
       </c>
       <c r="I6" s="7" t="s">
-        <v>148</v>
+        <v>59</v>
       </c>
       <c r="J6" s="7" t="s">
-        <v>147</v>
+        <v>58</v>
       </c>
       <c r="K6" s="7" t="s">
-        <v>147</v>
+        <v>58</v>
       </c>
     </row>
     <row r="7" spans="1:11">
@@ -5632,44 +5630,44 @@
         <v>5</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>117</v>
+        <v>28</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>118</v>
+        <v>29</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>147</v>
+        <v>58</v>
       </c>
       <c r="F7" s="7" t="s">
-        <v>148</v>
+        <v>59</v>
       </c>
       <c r="G7" s="7" t="s">
-        <v>147</v>
+        <v>58</v>
       </c>
       <c r="H7" s="7" t="s">
-        <v>148</v>
+        <v>59</v>
       </c>
       <c r="I7" s="7" t="s">
-        <v>147</v>
+        <v>58</v>
       </c>
       <c r="J7" s="7" t="s">
-        <v>147</v>
+        <v>58</v>
       </c>
       <c r="K7" s="7" t="s">
-        <v>147</v>
+        <v>58</v>
       </c>
     </row>
     <row r="11" spans="1:11">
       <c r="A11" s="4" t="s">
-        <v>119</v>
+        <v>30</v>
       </c>
     </row>
     <row r="12" spans="1:11">
       <c r="C12" s="5" t="s">
-        <v>136</v>
+        <v>47</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>137</v>
+        <v>48</v>
       </c>
     </row>
     <row r="13" spans="1:11">
@@ -5677,10 +5675,10 @@
         <v>1</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>120</v>
+        <v>31</v>
       </c>
       <c r="D13" s="7" t="s">
-        <v>121</v>
+        <v>32</v>
       </c>
     </row>
     <row r="14" spans="1:11">
@@ -5688,10 +5686,10 @@
         <v>2</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>122</v>
+        <v>33</v>
       </c>
       <c r="D14" s="7" t="s">
-        <v>123</v>
+        <v>34</v>
       </c>
     </row>
     <row r="15" spans="1:11">
@@ -5699,10 +5697,10 @@
         <v>3</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>124</v>
+        <v>35</v>
       </c>
       <c r="D15" s="7" t="s">
-        <v>125</v>
+        <v>36</v>
       </c>
     </row>
     <row r="16" spans="1:11">
@@ -5710,10 +5708,10 @@
         <v>4</v>
       </c>
       <c r="C16" s="7" t="s">
-        <v>126</v>
+        <v>37</v>
       </c>
       <c r="D16" s="7" t="s">
-        <v>127</v>
+        <v>38</v>
       </c>
     </row>
     <row r="17" spans="2:4">
@@ -5721,10 +5719,10 @@
         <v>5</v>
       </c>
       <c r="C17" s="7" t="s">
-        <v>128</v>
+        <v>39</v>
       </c>
       <c r="D17" s="7" t="s">
-        <v>22</v>
+        <v>127</v>
       </c>
     </row>
     <row r="18" spans="2:4">
@@ -5732,10 +5730,10 @@
         <v>6</v>
       </c>
       <c r="C18" s="7" t="s">
-        <v>23</v>
+        <v>128</v>
       </c>
       <c r="D18" s="7" t="s">
-        <v>24</v>
+        <v>129</v>
       </c>
     </row>
     <row r="19" spans="2:4">
@@ -5743,10 +5741,10 @@
         <v>7</v>
       </c>
       <c r="C19" s="7" t="s">
-        <v>25</v>
+        <v>130</v>
       </c>
       <c r="D19" s="7" t="s">
-        <v>26</v>
+        <v>131</v>
       </c>
     </row>
     <row r="20" spans="2:4">
@@ -5754,10 +5752,10 @@
         <v>8</v>
       </c>
       <c r="C20" s="7" t="s">
-        <v>21</v>
+        <v>126</v>
       </c>
       <c r="D20" s="7" t="s">
-        <v>20</v>
+        <v>125</v>
       </c>
     </row>
     <row r="21" spans="2:4">
@@ -5765,14 +5763,13 @@
         <v>9</v>
       </c>
       <c r="C21" s="7" t="s">
-        <v>19</v>
+        <v>124</v>
       </c>
       <c r="D21" s="7" t="s">
-        <v>18</v>
+        <v>123</v>
       </c>
     </row>
   </sheetData>
-  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
@@ -5788,8 +5785,8 @@
   <sheetPr published="0" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:Z28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="Q10" sqref="Q10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.625" defaultRowHeight="15"/>
@@ -5799,7 +5796,7 @@
   <sheetData>
     <row r="1" spans="1:26">
       <c r="A1" s="4" t="s">
-        <v>27</v>
+        <v>132</v>
       </c>
     </row>
     <row r="2" spans="1:26">
@@ -5867,7 +5864,7 @@
         <v>2020</v>
       </c>
       <c r="Z2" s="6" t="s">
-        <v>28</v>
+        <v>133</v>
       </c>
     </row>
     <row r="3" spans="1:26">
@@ -5876,7 +5873,7 @@
         <v>SBCC</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>29</v>
+        <v>134</v>
       </c>
       <c r="D3" s="8"/>
       <c r="E3" s="8"/>
@@ -5902,7 +5899,7 @@
       <c r="W3" s="8"/>
       <c r="X3" s="8"/>
       <c r="Y3" s="9" t="s">
-        <v>30</v>
+        <v>135</v>
       </c>
       <c r="Z3" s="8"/>
     </row>
@@ -5912,7 +5909,7 @@
         <v>SBCC</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>31</v>
+        <v>136</v>
       </c>
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
@@ -5938,7 +5935,7 @@
       <c r="W4" s="10"/>
       <c r="X4" s="10"/>
       <c r="Y4" s="9" t="s">
-        <v>30</v>
+        <v>135</v>
       </c>
       <c r="Z4" s="10"/>
     </row>
@@ -5948,7 +5945,7 @@
         <v>FSW programs</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>29</v>
+        <v>134</v>
       </c>
       <c r="D6" s="8"/>
       <c r="E6" s="8"/>
@@ -5974,7 +5971,7 @@
       <c r="W6" s="8"/>
       <c r="X6" s="8"/>
       <c r="Y6" s="9" t="s">
-        <v>30</v>
+        <v>135</v>
       </c>
       <c r="Z6" s="8"/>
     </row>
@@ -5984,7 +5981,7 @@
         <v>FSW programs</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>31</v>
+        <v>136</v>
       </c>
       <c r="D7" s="10"/>
       <c r="E7" s="10"/>
@@ -6010,7 +6007,7 @@
       <c r="W7" s="10"/>
       <c r="X7" s="10"/>
       <c r="Y7" s="9" t="s">
-        <v>30</v>
+        <v>135</v>
       </c>
       <c r="Z7" s="10"/>
     </row>
@@ -6020,7 +6017,7 @@
         <v>MSM programs</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>29</v>
+        <v>134</v>
       </c>
       <c r="D9" s="8"/>
       <c r="E9" s="8"/>
@@ -6035,8 +6032,8 @@
       <c r="N9" s="8"/>
       <c r="O9" s="8"/>
       <c r="P9" s="8"/>
-      <c r="Q9" s="8">
-        <v>4.9000000000000002E-2</v>
+      <c r="Q9" s="28">
+        <v>400000</v>
       </c>
       <c r="R9" s="8"/>
       <c r="S9" s="8"/>
@@ -6046,7 +6043,7 @@
       <c r="W9" s="8"/>
       <c r="X9" s="8"/>
       <c r="Y9" s="9" t="s">
-        <v>30</v>
+        <v>135</v>
       </c>
       <c r="Z9" s="8"/>
     </row>
@@ -6056,7 +6053,7 @@
         <v>MSM programs</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>31</v>
+        <v>136</v>
       </c>
       <c r="D10" s="10"/>
       <c r="E10" s="10"/>
@@ -6082,7 +6079,7 @@
       <c r="W10" s="10"/>
       <c r="X10" s="10"/>
       <c r="Y10" s="9" t="s">
-        <v>30</v>
+        <v>135</v>
       </c>
       <c r="Z10" s="10"/>
     </row>
@@ -6092,7 +6089,7 @@
         <v>HTC</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>29</v>
+        <v>134</v>
       </c>
       <c r="D12" s="8"/>
       <c r="E12" s="8"/>
@@ -6118,7 +6115,7 @@
       <c r="W12" s="8"/>
       <c r="X12" s="8"/>
       <c r="Y12" s="9" t="s">
-        <v>30</v>
+        <v>135</v>
       </c>
       <c r="Z12" s="8"/>
     </row>
@@ -6128,7 +6125,7 @@
         <v>HTC</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>31</v>
+        <v>136</v>
       </c>
       <c r="D13" s="10"/>
       <c r="E13" s="10"/>
@@ -6154,7 +6151,7 @@
       <c r="W13" s="10"/>
       <c r="X13" s="10"/>
       <c r="Y13" s="9" t="s">
-        <v>30</v>
+        <v>135</v>
       </c>
       <c r="Z13" s="10"/>
     </row>
@@ -6164,7 +6161,7 @@
         <v>ART</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>29</v>
+        <v>134</v>
       </c>
       <c r="D15" s="8"/>
       <c r="E15" s="8"/>
@@ -6190,7 +6187,7 @@
       <c r="W15" s="8"/>
       <c r="X15" s="8"/>
       <c r="Y15" s="9" t="s">
-        <v>30</v>
+        <v>135</v>
       </c>
       <c r="Z15" s="8"/>
     </row>
@@ -6200,7 +6197,7 @@
         <v>ART</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>31</v>
+        <v>136</v>
       </c>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
@@ -6226,7 +6223,7 @@
       <c r="W16" s="10"/>
       <c r="X16" s="10"/>
       <c r="Y16" s="9" t="s">
-        <v>30</v>
+        <v>135</v>
       </c>
       <c r="Z16" s="10"/>
     </row>
@@ -6236,7 +6233,7 @@
         <v>PMTCT</v>
       </c>
       <c r="C18" s="6" t="s">
-        <v>29</v>
+        <v>134</v>
       </c>
       <c r="D18" s="8"/>
       <c r="E18" s="8"/>
@@ -6262,7 +6259,7 @@
       <c r="W18" s="8"/>
       <c r="X18" s="8"/>
       <c r="Y18" s="9" t="s">
-        <v>30</v>
+        <v>135</v>
       </c>
       <c r="Z18" s="8"/>
     </row>
@@ -6272,7 +6269,7 @@
         <v>PMTCT</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>31</v>
+        <v>136</v>
       </c>
       <c r="D19" s="10"/>
       <c r="E19" s="10"/>
@@ -6298,7 +6295,7 @@
       <c r="W19" s="10"/>
       <c r="X19" s="10"/>
       <c r="Y19" s="9" t="s">
-        <v>30</v>
+        <v>135</v>
       </c>
       <c r="Z19" s="10"/>
     </row>
@@ -6308,7 +6305,7 @@
         <v>MGMT</v>
       </c>
       <c r="C21" s="6" t="s">
-        <v>29</v>
+        <v>134</v>
       </c>
       <c r="D21" s="8"/>
       <c r="E21" s="8"/>
@@ -6332,7 +6329,7 @@
       <c r="W21" s="8"/>
       <c r="X21" s="8"/>
       <c r="Y21" s="9" t="s">
-        <v>30</v>
+        <v>135</v>
       </c>
       <c r="Z21" s="8"/>
     </row>
@@ -6342,7 +6339,7 @@
         <v>MGMT</v>
       </c>
       <c r="C22" s="6" t="s">
-        <v>31</v>
+        <v>136</v>
       </c>
       <c r="D22" s="10"/>
       <c r="E22" s="10"/>
@@ -6368,7 +6365,7 @@
       <c r="W22" s="10"/>
       <c r="X22" s="10"/>
       <c r="Y22" s="9" t="s">
-        <v>30</v>
+        <v>135</v>
       </c>
       <c r="Z22" s="10"/>
     </row>
@@ -6378,7 +6375,7 @@
         <v>ENV</v>
       </c>
       <c r="C24" s="6" t="s">
-        <v>29</v>
+        <v>134</v>
       </c>
       <c r="D24" s="8"/>
       <c r="E24" s="8"/>
@@ -6402,7 +6399,7 @@
       <c r="W24" s="8"/>
       <c r="X24" s="8"/>
       <c r="Y24" s="9" t="s">
-        <v>30</v>
+        <v>135</v>
       </c>
       <c r="Z24" s="8"/>
     </row>
@@ -6412,7 +6409,7 @@
         <v>ENV</v>
       </c>
       <c r="C25" s="6" t="s">
-        <v>31</v>
+        <v>136</v>
       </c>
       <c r="D25" s="10"/>
       <c r="E25" s="10"/>
@@ -6438,7 +6435,7 @@
       <c r="W25" s="10"/>
       <c r="X25" s="10"/>
       <c r="Y25" s="9" t="s">
-        <v>30</v>
+        <v>135</v>
       </c>
       <c r="Z25" s="10"/>
     </row>
@@ -6448,7 +6445,7 @@
         <v>Other</v>
       </c>
       <c r="C27" s="6" t="s">
-        <v>29</v>
+        <v>134</v>
       </c>
       <c r="D27" s="8"/>
       <c r="E27" s="8"/>
@@ -6472,7 +6469,7 @@
       <c r="W27" s="8"/>
       <c r="X27" s="8"/>
       <c r="Y27" s="9" t="s">
-        <v>30</v>
+        <v>135</v>
       </c>
       <c r="Z27" s="8"/>
     </row>
@@ -6482,7 +6479,7 @@
         <v>Other</v>
       </c>
       <c r="C28" s="6" t="s">
-        <v>31</v>
+        <v>136</v>
       </c>
       <c r="D28" s="10"/>
       <c r="E28" s="10"/>
@@ -6508,12 +6505,11 @@
       <c r="W28" s="10"/>
       <c r="X28" s="10"/>
       <c r="Y28" s="9" t="s">
-        <v>30</v>
+        <v>135</v>
       </c>
       <c r="Z28" s="10"/>
     </row>
   </sheetData>
-  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
@@ -6538,7 +6534,7 @@
   <sheetData>
     <row r="1" spans="1:26">
       <c r="A1" s="4" t="s">
-        <v>32</v>
+        <v>137</v>
       </c>
     </row>
     <row r="2" spans="1:26">
@@ -6606,7 +6602,7 @@
         <v>2020</v>
       </c>
       <c r="Z2" s="6" t="s">
-        <v>28</v>
+        <v>133</v>
       </c>
     </row>
     <row r="3" spans="1:26">
@@ -6615,7 +6611,7 @@
         <v>FSW</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>33</v>
+        <v>138</v>
       </c>
       <c r="D3" s="10"/>
       <c r="E3" s="10"/>
@@ -6639,7 +6635,7 @@
       <c r="W3" s="10"/>
       <c r="X3" s="10"/>
       <c r="Y3" s="9" t="s">
-        <v>30</v>
+        <v>135</v>
       </c>
       <c r="Z3" s="10"/>
     </row>
@@ -6649,7 +6645,7 @@
         <v>FSW</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>34</v>
+        <v>139</v>
       </c>
       <c r="D4" s="13">
         <v>139172.68199999997</v>
@@ -6695,7 +6691,7 @@
       <c r="W4" s="10"/>
       <c r="X4" s="10"/>
       <c r="Y4" s="9" t="s">
-        <v>30</v>
+        <v>135</v>
       </c>
       <c r="Z4" s="10"/>
     </row>
@@ -6705,7 +6701,7 @@
         <v>FSW</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>35</v>
+        <v>140</v>
       </c>
       <c r="D5" s="10"/>
       <c r="E5" s="10"/>
@@ -6729,7 +6725,7 @@
       <c r="W5" s="10"/>
       <c r="X5" s="10"/>
       <c r="Y5" s="9" t="s">
-        <v>30</v>
+        <v>135</v>
       </c>
       <c r="Z5" s="10"/>
     </row>
@@ -6739,7 +6735,7 @@
         <v>Clients</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>33</v>
+        <v>138</v>
       </c>
       <c r="D7" s="10"/>
       <c r="E7" s="10"/>
@@ -6763,7 +6759,7 @@
       <c r="W7" s="10"/>
       <c r="X7" s="10"/>
       <c r="Y7" s="9" t="s">
-        <v>30</v>
+        <v>135</v>
       </c>
       <c r="Z7" s="10"/>
     </row>
@@ -6773,7 +6769,7 @@
         <v>Clients</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>34</v>
+        <v>139</v>
       </c>
       <c r="D8" s="13">
         <v>979330.74050000007</v>
@@ -6819,7 +6815,7 @@
       <c r="W8" s="10"/>
       <c r="X8" s="10"/>
       <c r="Y8" s="9" t="s">
-        <v>30</v>
+        <v>135</v>
       </c>
       <c r="Z8" s="10"/>
     </row>
@@ -6829,7 +6825,7 @@
         <v>Clients</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>35</v>
+        <v>140</v>
       </c>
       <c r="D9" s="10"/>
       <c r="E9" s="10"/>
@@ -6853,7 +6849,7 @@
       <c r="W9" s="10"/>
       <c r="X9" s="10"/>
       <c r="Y9" s="9" t="s">
-        <v>30</v>
+        <v>135</v>
       </c>
       <c r="Z9" s="10"/>
     </row>
@@ -6863,7 +6859,7 @@
         <v>MSM</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>33</v>
+        <v>138</v>
       </c>
       <c r="D11" s="10"/>
       <c r="E11" s="10"/>
@@ -6887,7 +6883,7 @@
       <c r="W11" s="10"/>
       <c r="X11" s="10"/>
       <c r="Y11" s="9" t="s">
-        <v>30</v>
+        <v>135</v>
       </c>
       <c r="Z11" s="10"/>
     </row>
@@ -6897,7 +6893,7 @@
         <v>MSM</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>34</v>
+        <v>139</v>
       </c>
       <c r="D12" s="13">
         <v>96306.278800000015</v>
@@ -6943,7 +6939,7 @@
       <c r="W12" s="10"/>
       <c r="X12" s="10"/>
       <c r="Y12" s="9" t="s">
-        <v>30</v>
+        <v>135</v>
       </c>
       <c r="Z12" s="10"/>
     </row>
@@ -6953,7 +6949,7 @@
         <v>MSM</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>35</v>
+        <v>140</v>
       </c>
       <c r="D13" s="10"/>
       <c r="E13" s="10"/>
@@ -6977,7 +6973,7 @@
       <c r="W13" s="10"/>
       <c r="X13" s="10"/>
       <c r="Y13" s="9" t="s">
-        <v>30</v>
+        <v>135</v>
       </c>
       <c r="Z13" s="10"/>
     </row>
@@ -6987,7 +6983,7 @@
         <v>Males 15-49</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>33</v>
+        <v>138</v>
       </c>
       <c r="D15" s="10"/>
       <c r="E15" s="10"/>
@@ -7011,7 +7007,7 @@
       <c r="W15" s="10"/>
       <c r="X15" s="10"/>
       <c r="Y15" s="9" t="s">
-        <v>30</v>
+        <v>135</v>
       </c>
       <c r="Z15" s="10"/>
     </row>
@@ -7021,7 +7017,7 @@
         <v>Males 15-49</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>34</v>
+        <v>139</v>
       </c>
       <c r="D16" s="10">
         <v>5431543.9807000002</v>
@@ -7067,7 +7063,7 @@
       <c r="W16" s="10"/>
       <c r="X16" s="10"/>
       <c r="Y16" s="9" t="s">
-        <v>30</v>
+        <v>135</v>
       </c>
       <c r="Z16" s="10"/>
     </row>
@@ -7077,7 +7073,7 @@
         <v>Males 15-49</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>35</v>
+        <v>140</v>
       </c>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
@@ -7101,7 +7097,7 @@
       <c r="W17" s="10"/>
       <c r="X17" s="10"/>
       <c r="Y17" s="9" t="s">
-        <v>30</v>
+        <v>135</v>
       </c>
       <c r="Z17" s="10"/>
     </row>
@@ -7111,7 +7107,7 @@
         <v>Females 15-49</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>33</v>
+        <v>138</v>
       </c>
       <c r="D19" s="10"/>
       <c r="E19" s="10"/>
@@ -7135,7 +7131,7 @@
       <c r="W19" s="10"/>
       <c r="X19" s="10"/>
       <c r="Y19" s="9" t="s">
-        <v>30</v>
+        <v>135</v>
       </c>
       <c r="Z19" s="10"/>
     </row>
@@ -7145,7 +7141,7 @@
         <v>Females 15-49</v>
       </c>
       <c r="C20" s="6" t="s">
-        <v>34</v>
+        <v>139</v>
       </c>
       <c r="D20" s="10">
         <v>6333671.4559585694</v>
@@ -7191,7 +7187,7 @@
       <c r="W20" s="10"/>
       <c r="X20" s="10"/>
       <c r="Y20" s="9" t="s">
-        <v>30</v>
+        <v>135</v>
       </c>
       <c r="Z20" s="10"/>
     </row>
@@ -7201,7 +7197,7 @@
         <v>Females 15-49</v>
       </c>
       <c r="C21" s="6" t="s">
-        <v>35</v>
+        <v>140</v>
       </c>
       <c r="D21" s="10"/>
       <c r="E21" s="10"/>
@@ -7225,13 +7221,13 @@
       <c r="W21" s="10"/>
       <c r="X21" s="10"/>
       <c r="Y21" s="9" t="s">
-        <v>30</v>
+        <v>135</v>
       </c>
       <c r="Z21" s="10"/>
     </row>
     <row r="26" spans="1:26">
       <c r="A26" s="4" t="s">
-        <v>36</v>
+        <v>141</v>
       </c>
     </row>
     <row r="27" spans="1:26">
@@ -7299,7 +7295,7 @@
         <v>2020</v>
       </c>
       <c r="Z27" s="6" t="s">
-        <v>28</v>
+        <v>133</v>
       </c>
     </row>
     <row r="28" spans="1:26">
@@ -7308,7 +7304,7 @@
         <v>FSW</v>
       </c>
       <c r="C28" s="6" t="s">
-        <v>33</v>
+        <v>138</v>
       </c>
       <c r="D28" s="8"/>
       <c r="E28" s="8"/>
@@ -7332,7 +7328,7 @@
       <c r="W28" s="8"/>
       <c r="X28" s="8"/>
       <c r="Y28" s="9" t="s">
-        <v>30</v>
+        <v>135</v>
       </c>
       <c r="Z28" s="8"/>
     </row>
@@ -7342,7 +7338,7 @@
         <v>FSW</v>
       </c>
       <c r="C29" s="6" t="s">
-        <v>34</v>
+        <v>139</v>
       </c>
       <c r="D29" s="8"/>
       <c r="E29" s="8"/>
@@ -7368,7 +7364,7 @@
       <c r="W29" s="8"/>
       <c r="X29" s="8"/>
       <c r="Y29" s="9" t="s">
-        <v>30</v>
+        <v>135</v>
       </c>
       <c r="Z29" s="8"/>
     </row>
@@ -7378,7 +7374,7 @@
         <v>FSW</v>
       </c>
       <c r="C30" s="6" t="s">
-        <v>35</v>
+        <v>140</v>
       </c>
       <c r="D30" s="8"/>
       <c r="E30" s="8"/>
@@ -7402,7 +7398,7 @@
       <c r="W30" s="8"/>
       <c r="X30" s="8"/>
       <c r="Y30" s="9" t="s">
-        <v>30</v>
+        <v>135</v>
       </c>
       <c r="Z30" s="8"/>
     </row>
@@ -7412,7 +7408,7 @@
         <v>Clients</v>
       </c>
       <c r="C32" s="6" t="s">
-        <v>33</v>
+        <v>138</v>
       </c>
       <c r="D32" s="8"/>
       <c r="E32" s="8"/>
@@ -7436,7 +7432,7 @@
       <c r="W32" s="8"/>
       <c r="X32" s="8"/>
       <c r="Y32" s="9" t="s">
-        <v>30</v>
+        <v>135</v>
       </c>
       <c r="Z32" s="8"/>
     </row>
@@ -7446,7 +7442,7 @@
         <v>Clients</v>
       </c>
       <c r="C33" s="6" t="s">
-        <v>34</v>
+        <v>139</v>
       </c>
       <c r="D33" s="8"/>
       <c r="E33" s="8"/>
@@ -7472,7 +7468,7 @@
       <c r="W33" s="8"/>
       <c r="X33" s="8"/>
       <c r="Y33" s="9" t="s">
-        <v>30</v>
+        <v>135</v>
       </c>
       <c r="Z33" s="8"/>
     </row>
@@ -7482,7 +7478,7 @@
         <v>Clients</v>
       </c>
       <c r="C34" s="6" t="s">
-        <v>35</v>
+        <v>140</v>
       </c>
       <c r="D34" s="8"/>
       <c r="E34" s="8"/>
@@ -7506,7 +7502,7 @@
       <c r="W34" s="8"/>
       <c r="X34" s="8"/>
       <c r="Y34" s="9" t="s">
-        <v>30</v>
+        <v>135</v>
       </c>
       <c r="Z34" s="8"/>
     </row>
@@ -7516,7 +7512,7 @@
         <v>MSM</v>
       </c>
       <c r="C36" s="6" t="s">
-        <v>33</v>
+        <v>138</v>
       </c>
       <c r="D36" s="8"/>
       <c r="E36" s="8"/>
@@ -7540,7 +7536,7 @@
       <c r="W36" s="8"/>
       <c r="X36" s="8"/>
       <c r="Y36" s="9" t="s">
-        <v>30</v>
+        <v>135</v>
       </c>
       <c r="Z36" s="8"/>
     </row>
@@ -7550,7 +7546,7 @@
         <v>MSM</v>
       </c>
       <c r="C37" s="6" t="s">
-        <v>34</v>
+        <v>139</v>
       </c>
       <c r="D37" s="8"/>
       <c r="E37" s="8"/>
@@ -7576,7 +7572,7 @@
       <c r="W37" s="8"/>
       <c r="X37" s="8"/>
       <c r="Y37" s="9" t="s">
-        <v>30</v>
+        <v>135</v>
       </c>
       <c r="Z37" s="8"/>
     </row>
@@ -7586,7 +7582,7 @@
         <v>MSM</v>
       </c>
       <c r="C38" s="6" t="s">
-        <v>35</v>
+        <v>140</v>
       </c>
       <c r="D38" s="8"/>
       <c r="E38" s="8"/>
@@ -7610,7 +7606,7 @@
       <c r="W38" s="8"/>
       <c r="X38" s="8"/>
       <c r="Y38" s="9" t="s">
-        <v>30</v>
+        <v>135</v>
       </c>
       <c r="Z38" s="8"/>
     </row>
@@ -7620,7 +7616,7 @@
         <v>Males 15-49</v>
       </c>
       <c r="C40" s="6" t="s">
-        <v>33</v>
+        <v>138</v>
       </c>
       <c r="D40" s="8"/>
       <c r="E40" s="8"/>
@@ -7644,7 +7640,7 @@
       <c r="W40" s="8"/>
       <c r="X40" s="8"/>
       <c r="Y40" s="9" t="s">
-        <v>30</v>
+        <v>135</v>
       </c>
       <c r="Z40" s="8"/>
     </row>
@@ -7654,7 +7650,7 @@
         <v>Males 15-49</v>
       </c>
       <c r="C41" s="6" t="s">
-        <v>34</v>
+        <v>139</v>
       </c>
       <c r="D41" s="8"/>
       <c r="E41" s="8"/>
@@ -7684,7 +7680,7 @@
       <c r="W41" s="8"/>
       <c r="X41" s="8"/>
       <c r="Y41" s="9" t="s">
-        <v>30</v>
+        <v>135</v>
       </c>
       <c r="Z41" s="8"/>
     </row>
@@ -7694,7 +7690,7 @@
         <v>Males 15-49</v>
       </c>
       <c r="C42" s="6" t="s">
-        <v>35</v>
+        <v>140</v>
       </c>
       <c r="D42" s="8"/>
       <c r="E42" s="8"/>
@@ -7718,7 +7714,7 @@
       <c r="W42" s="8"/>
       <c r="X42" s="8"/>
       <c r="Y42" s="9" t="s">
-        <v>30</v>
+        <v>135</v>
       </c>
       <c r="Z42" s="8"/>
     </row>
@@ -7728,7 +7724,7 @@
         <v>Females 15-49</v>
       </c>
       <c r="C44" s="6" t="s">
-        <v>33</v>
+        <v>138</v>
       </c>
       <c r="D44" s="8"/>
       <c r="E44" s="8"/>
@@ -7752,7 +7748,7 @@
       <c r="W44" s="8"/>
       <c r="X44" s="8"/>
       <c r="Y44" s="9" t="s">
-        <v>30</v>
+        <v>135</v>
       </c>
       <c r="Z44" s="8"/>
     </row>
@@ -7762,7 +7758,7 @@
         <v>Females 15-49</v>
       </c>
       <c r="C45" s="6" t="s">
-        <v>34</v>
+        <v>139</v>
       </c>
       <c r="D45" s="8"/>
       <c r="E45" s="8"/>
@@ -7792,7 +7788,7 @@
       <c r="W45" s="8"/>
       <c r="X45" s="8"/>
       <c r="Y45" s="9" t="s">
-        <v>30</v>
+        <v>135</v>
       </c>
       <c r="Z45" s="8"/>
     </row>
@@ -7802,7 +7798,7 @@
         <v>Females 15-49</v>
       </c>
       <c r="C46" s="6" t="s">
-        <v>35</v>
+        <v>140</v>
       </c>
       <c r="D46" s="8"/>
       <c r="E46" s="8"/>
@@ -7826,12 +7822,11 @@
       <c r="W46" s="8"/>
       <c r="X46" s="8"/>
       <c r="Y46" s="9" t="s">
-        <v>30</v>
+        <v>135</v>
       </c>
       <c r="Z46" s="8"/>
     </row>
   </sheetData>
-  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
@@ -7856,7 +7851,7 @@
   <sheetData>
     <row r="1" spans="1:25">
       <c r="A1" s="4" t="s">
-        <v>37</v>
+        <v>142</v>
       </c>
     </row>
     <row r="2" spans="1:25">
@@ -7924,12 +7919,12 @@
         <v>2020</v>
       </c>
       <c r="Y2" s="6" t="s">
-        <v>28</v>
+        <v>133</v>
       </c>
     </row>
     <row r="3" spans="1:25">
       <c r="B3" s="6" t="s">
-        <v>38</v>
+        <v>143</v>
       </c>
       <c r="C3" s="11"/>
       <c r="D3" s="11"/>
@@ -7967,13 +7962,13 @@
       <c r="V3" s="11"/>
       <c r="W3" s="11"/>
       <c r="X3" s="9" t="s">
-        <v>30</v>
+        <v>135</v>
       </c>
       <c r="Y3" s="11"/>
     </row>
     <row r="7" spans="1:25">
       <c r="A7" s="4" t="s">
-        <v>39</v>
+        <v>144</v>
       </c>
     </row>
     <row r="8" spans="1:25">
@@ -8041,12 +8036,12 @@
         <v>2020</v>
       </c>
       <c r="Y8" s="6" t="s">
-        <v>28</v>
+        <v>133</v>
       </c>
     </row>
     <row r="9" spans="1:25">
       <c r="B9" s="6" t="s">
-        <v>38</v>
+        <v>143</v>
       </c>
       <c r="C9" s="11"/>
       <c r="D9" s="11"/>
@@ -8072,13 +8067,13 @@
       <c r="V9" s="11"/>
       <c r="W9" s="11"/>
       <c r="X9" s="9" t="s">
-        <v>30</v>
+        <v>135</v>
       </c>
       <c r="Y9" s="11"/>
     </row>
     <row r="13" spans="1:25">
       <c r="A13" s="4" t="s">
-        <v>40</v>
+        <v>145</v>
       </c>
     </row>
     <row r="14" spans="1:25">
@@ -8146,12 +8141,12 @@
         <v>2020</v>
       </c>
       <c r="Y14" s="6" t="s">
-        <v>28</v>
+        <v>133</v>
       </c>
     </row>
     <row r="15" spans="1:25">
       <c r="B15" s="6" t="s">
-        <v>38</v>
+        <v>143</v>
       </c>
       <c r="C15" s="16">
         <v>3121.27</v>
@@ -8203,13 +8198,13 @@
       <c r="V15" s="11"/>
       <c r="W15" s="11"/>
       <c r="X15" s="9" t="s">
-        <v>30</v>
+        <v>135</v>
       </c>
       <c r="Y15" s="11"/>
     </row>
     <row r="19" spans="1:25">
       <c r="A19" s="4" t="s">
-        <v>41</v>
+        <v>146</v>
       </c>
     </row>
     <row r="20" spans="1:25">
@@ -8277,12 +8272,12 @@
         <v>2020</v>
       </c>
       <c r="Y20" s="6" t="s">
-        <v>28</v>
+        <v>133</v>
       </c>
     </row>
     <row r="21" spans="1:25">
       <c r="B21" s="6" t="s">
-        <v>38</v>
+        <v>143</v>
       </c>
       <c r="C21" s="11">
         <v>0.11</v>
@@ -8334,13 +8329,13 @@
       <c r="V21" s="11"/>
       <c r="W21" s="11"/>
       <c r="X21" s="9" t="s">
-        <v>30</v>
+        <v>135</v>
       </c>
       <c r="Y21" s="11"/>
     </row>
     <row r="25" spans="1:25">
       <c r="A25" s="4" t="s">
-        <v>42</v>
+        <v>147</v>
       </c>
     </row>
     <row r="26" spans="1:25">
@@ -8408,12 +8403,12 @@
         <v>2020</v>
       </c>
       <c r="Y26" s="6" t="s">
-        <v>28</v>
+        <v>133</v>
       </c>
     </row>
     <row r="27" spans="1:25">
       <c r="B27" s="6" t="s">
-        <v>38</v>
+        <v>143</v>
       </c>
       <c r="C27" s="16">
         <v>714</v>
@@ -8465,13 +8460,13 @@
       <c r="V27" s="11"/>
       <c r="W27" s="11"/>
       <c r="X27" s="9" t="s">
-        <v>30</v>
+        <v>135</v>
       </c>
       <c r="Y27" s="11"/>
     </row>
     <row r="31" spans="1:25">
       <c r="A31" s="4" t="s">
-        <v>43</v>
+        <v>148</v>
       </c>
     </row>
     <row r="32" spans="1:25">
@@ -8539,12 +8534,12 @@
         <v>2020</v>
       </c>
       <c r="Y32" s="6" t="s">
-        <v>28</v>
+        <v>133</v>
       </c>
     </row>
     <row r="33" spans="2:25">
       <c r="B33" s="6" t="s">
-        <v>38</v>
+        <v>143</v>
       </c>
       <c r="C33" s="11"/>
       <c r="D33" s="11"/>
@@ -8568,12 +8563,11 @@
       <c r="V33" s="11"/>
       <c r="W33" s="11"/>
       <c r="X33" s="9" t="s">
-        <v>30</v>
+        <v>135</v>
       </c>
       <c r="Y33" s="11"/>
     </row>
   </sheetData>
-  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
@@ -8598,7 +8592,7 @@
   <sheetData>
     <row r="1" spans="1:25">
       <c r="A1" s="4" t="s">
-        <v>44</v>
+        <v>149</v>
       </c>
     </row>
     <row r="2" spans="1:25">
@@ -8666,7 +8660,7 @@
         <v>2020</v>
       </c>
       <c r="Y2" s="6" t="s">
-        <v>28</v>
+        <v>133</v>
       </c>
     </row>
     <row r="3" spans="1:25">
@@ -8696,7 +8690,7 @@
       <c r="V3" s="8"/>
       <c r="W3" s="8"/>
       <c r="X3" s="9" t="s">
-        <v>30</v>
+        <v>135</v>
       </c>
       <c r="Y3" s="8">
         <v>0.01</v>
@@ -8729,7 +8723,7 @@
       <c r="V4" s="8"/>
       <c r="W4" s="8"/>
       <c r="X4" s="9" t="s">
-        <v>30</v>
+        <v>135</v>
       </c>
       <c r="Y4" s="8">
         <v>0.01</v>
@@ -8762,7 +8756,7 @@
       <c r="V5" s="8"/>
       <c r="W5" s="8"/>
       <c r="X5" s="9" t="s">
-        <v>30</v>
+        <v>135</v>
       </c>
       <c r="Y5" s="8">
         <v>0.01</v>
@@ -8795,7 +8789,7 @@
       <c r="V6" s="8"/>
       <c r="W6" s="8"/>
       <c r="X6" s="9" t="s">
-        <v>30</v>
+        <v>135</v>
       </c>
       <c r="Y6" s="8">
         <v>0.01</v>
@@ -8828,7 +8822,7 @@
       <c r="V7" s="8"/>
       <c r="W7" s="8"/>
       <c r="X7" s="9" t="s">
-        <v>30</v>
+        <v>135</v>
       </c>
       <c r="Y7" s="8">
         <v>0.01</v>
@@ -8836,7 +8830,7 @@
     </row>
     <row r="11" spans="1:25">
       <c r="A11" s="4" t="s">
-        <v>45</v>
+        <v>150</v>
       </c>
     </row>
     <row r="12" spans="1:25">
@@ -8904,7 +8898,7 @@
         <v>2020</v>
       </c>
       <c r="Y12" s="6" t="s">
-        <v>28</v>
+        <v>133</v>
       </c>
     </row>
     <row r="13" spans="1:25">
@@ -8936,7 +8930,7 @@
       <c r="V13" s="8"/>
       <c r="W13" s="8"/>
       <c r="X13" s="9" t="s">
-        <v>30</v>
+        <v>135</v>
       </c>
       <c r="Y13" s="8"/>
     </row>
@@ -8967,7 +8961,7 @@
       <c r="V14" s="8"/>
       <c r="W14" s="8"/>
       <c r="X14" s="9" t="s">
-        <v>30</v>
+        <v>135</v>
       </c>
       <c r="Y14" s="8">
         <v>0.02</v>
@@ -9002,7 +8996,7 @@
       <c r="V15" s="8"/>
       <c r="W15" s="8"/>
       <c r="X15" s="9" t="s">
-        <v>30</v>
+        <v>135</v>
       </c>
       <c r="Y15" s="8"/>
     </row>
@@ -9033,7 +9027,7 @@
       <c r="V16" s="8"/>
       <c r="W16" s="8"/>
       <c r="X16" s="9" t="s">
-        <v>30</v>
+        <v>135</v>
       </c>
       <c r="Y16" s="8">
         <v>0.01</v>
@@ -9066,7 +9060,7 @@
       <c r="V17" s="8"/>
       <c r="W17" s="8"/>
       <c r="X17" s="9" t="s">
-        <v>30</v>
+        <v>135</v>
       </c>
       <c r="Y17" s="8">
         <v>0.01</v>
@@ -9074,7 +9068,7 @@
     </row>
     <row r="21" spans="1:25">
       <c r="A21" s="4" t="s">
-        <v>46</v>
+        <v>151</v>
       </c>
     </row>
     <row r="22" spans="1:25">
@@ -9142,7 +9136,7 @@
         <v>2020</v>
       </c>
       <c r="Y22" s="6" t="s">
-        <v>28</v>
+        <v>133</v>
       </c>
     </row>
     <row r="23" spans="1:25">
@@ -9174,7 +9168,7 @@
       <c r="V23" s="8"/>
       <c r="W23" s="8"/>
       <c r="X23" s="9" t="s">
-        <v>30</v>
+        <v>135</v>
       </c>
       <c r="Y23" s="8"/>
     </row>
@@ -9205,7 +9199,7 @@
       <c r="V24" s="8"/>
       <c r="W24" s="8"/>
       <c r="X24" s="9" t="s">
-        <v>30</v>
+        <v>135</v>
       </c>
       <c r="Y24" s="8">
         <v>0.05</v>
@@ -9240,7 +9234,7 @@
       <c r="V25" s="8"/>
       <c r="W25" s="8"/>
       <c r="X25" s="9" t="s">
-        <v>30</v>
+        <v>135</v>
       </c>
       <c r="Y25" s="8"/>
     </row>
@@ -9271,7 +9265,7 @@
       <c r="V26" s="8"/>
       <c r="W26" s="8"/>
       <c r="X26" s="9" t="s">
-        <v>30</v>
+        <v>135</v>
       </c>
       <c r="Y26" s="8">
         <v>0.01</v>
@@ -9304,7 +9298,7 @@
       <c r="V27" s="8"/>
       <c r="W27" s="8"/>
       <c r="X27" s="9" t="s">
-        <v>30</v>
+        <v>135</v>
       </c>
       <c r="Y27" s="8">
         <v>0.02</v>
@@ -9312,7 +9306,7 @@
     </row>
     <row r="31" spans="1:25">
       <c r="A31" s="4" t="s">
-        <v>47</v>
+        <v>152</v>
       </c>
     </row>
     <row r="32" spans="1:25">
@@ -9380,7 +9374,7 @@
         <v>2020</v>
       </c>
       <c r="Y32" s="6" t="s">
-        <v>28</v>
+        <v>133</v>
       </c>
     </row>
     <row r="33" spans="2:25">
@@ -9413,7 +9407,7 @@
       <c r="V33" s="8"/>
       <c r="W33" s="8"/>
       <c r="X33" s="9" t="s">
-        <v>30</v>
+        <v>135</v>
       </c>
       <c r="Y33" s="8"/>
     </row>
@@ -9447,7 +9441,7 @@
       <c r="V34" s="8"/>
       <c r="W34" s="8"/>
       <c r="X34" s="9" t="s">
-        <v>30</v>
+        <v>135</v>
       </c>
       <c r="Y34" s="8"/>
     </row>
@@ -9481,7 +9475,7 @@
       <c r="V35" s="8"/>
       <c r="W35" s="8"/>
       <c r="X35" s="9" t="s">
-        <v>30</v>
+        <v>135</v>
       </c>
       <c r="Y35" s="8"/>
     </row>
@@ -9515,7 +9509,7 @@
       <c r="V36" s="8"/>
       <c r="W36" s="8"/>
       <c r="X36" s="9" t="s">
-        <v>30</v>
+        <v>135</v>
       </c>
       <c r="Y36" s="8"/>
     </row>
@@ -9549,12 +9543,11 @@
       <c r="V37" s="8"/>
       <c r="W37" s="8"/>
       <c r="X37" s="9" t="s">
-        <v>30</v>
+        <v>135</v>
       </c>
       <c r="Y37" s="8"/>
     </row>
   </sheetData>
-  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
@@ -9579,7 +9572,7 @@
   <sheetData>
     <row r="1" spans="1:25">
       <c r="A1" s="4" t="s">
-        <v>150</v>
+        <v>61</v>
       </c>
     </row>
     <row r="2" spans="1:25">
@@ -9647,7 +9640,7 @@
         <v>2020</v>
       </c>
       <c r="Y2" s="6" t="s">
-        <v>28</v>
+        <v>133</v>
       </c>
     </row>
     <row r="3" spans="1:25">
@@ -9681,7 +9674,7 @@
       <c r="V3" s="12"/>
       <c r="W3" s="12"/>
       <c r="X3" s="9" t="s">
-        <v>30</v>
+        <v>135</v>
       </c>
       <c r="Y3" s="12"/>
     </row>
@@ -9714,7 +9707,7 @@
       <c r="V4" s="12"/>
       <c r="W4" s="12"/>
       <c r="X4" s="9" t="s">
-        <v>30</v>
+        <v>135</v>
       </c>
       <c r="Y4" s="12"/>
     </row>
@@ -9747,7 +9740,7 @@
       <c r="V5" s="12"/>
       <c r="W5" s="12"/>
       <c r="X5" s="9" t="s">
-        <v>30</v>
+        <v>135</v>
       </c>
       <c r="Y5" s="12"/>
     </row>
@@ -9780,7 +9773,7 @@
       <c r="V6" s="12"/>
       <c r="W6" s="12"/>
       <c r="X6" s="9" t="s">
-        <v>30</v>
+        <v>135</v>
       </c>
       <c r="Y6" s="12"/>
     </row>
@@ -9813,13 +9806,13 @@
       <c r="V7" s="12"/>
       <c r="W7" s="12"/>
       <c r="X7" s="9" t="s">
-        <v>30</v>
+        <v>135</v>
       </c>
       <c r="Y7" s="12"/>
     </row>
     <row r="11" spans="1:25">
       <c r="A11" s="4" t="s">
-        <v>151</v>
+        <v>62</v>
       </c>
     </row>
     <row r="12" spans="1:25">
@@ -9887,12 +9880,12 @@
         <v>2020</v>
       </c>
       <c r="Y12" s="6" t="s">
-        <v>28</v>
+        <v>133</v>
       </c>
     </row>
     <row r="13" spans="1:25">
       <c r="B13" s="6" t="s">
-        <v>152</v>
+        <v>63</v>
       </c>
       <c r="C13" s="7"/>
       <c r="D13" s="7"/>
@@ -9918,13 +9911,13 @@
       <c r="V13" s="7"/>
       <c r="W13" s="7"/>
       <c r="X13" s="9" t="s">
-        <v>30</v>
+        <v>135</v>
       </c>
       <c r="Y13" s="7"/>
     </row>
     <row r="17" spans="1:25">
       <c r="A17" s="4" t="s">
-        <v>153</v>
+        <v>64</v>
       </c>
     </row>
     <row r="18" spans="1:25">
@@ -9992,12 +9985,12 @@
         <v>2020</v>
       </c>
       <c r="Y18" s="6" t="s">
-        <v>28</v>
+        <v>133</v>
       </c>
     </row>
     <row r="19" spans="1:25">
       <c r="B19" s="6" t="s">
-        <v>38</v>
+        <v>143</v>
       </c>
       <c r="C19" s="7"/>
       <c r="D19" s="7"/>
@@ -10033,13 +10026,13 @@
       <c r="V19" s="7"/>
       <c r="W19" s="7"/>
       <c r="X19" s="9" t="s">
-        <v>30</v>
+        <v>135</v>
       </c>
       <c r="Y19" s="7"/>
     </row>
     <row r="23" spans="1:25">
       <c r="A23" s="4" t="s">
-        <v>154</v>
+        <v>65</v>
       </c>
     </row>
     <row r="24" spans="1:25">
@@ -10107,12 +10100,12 @@
         <v>2020</v>
       </c>
       <c r="Y24" s="6" t="s">
-        <v>28</v>
+        <v>133</v>
       </c>
     </row>
     <row r="25" spans="1:25">
       <c r="B25" s="6" t="s">
-        <v>38</v>
+        <v>143</v>
       </c>
       <c r="C25" s="7"/>
       <c r="D25" s="7"/>
@@ -10148,13 +10141,13 @@
       <c r="V25" s="7"/>
       <c r="W25" s="7"/>
       <c r="X25" s="9" t="s">
-        <v>30</v>
+        <v>135</v>
       </c>
       <c r="Y25" s="7"/>
     </row>
     <row r="29" spans="1:25">
       <c r="A29" s="4" t="s">
-        <v>155</v>
+        <v>66</v>
       </c>
     </row>
     <row r="30" spans="1:25">
@@ -10222,12 +10215,12 @@
         <v>2020</v>
       </c>
       <c r="Y30" s="6" t="s">
-        <v>28</v>
+        <v>133</v>
       </c>
     </row>
     <row r="31" spans="1:25">
       <c r="B31" s="6" t="s">
-        <v>38</v>
+        <v>143</v>
       </c>
       <c r="C31" s="7"/>
       <c r="D31" s="7"/>
@@ -10273,13 +10266,13 @@
       <c r="V31" s="7"/>
       <c r="W31" s="7"/>
       <c r="X31" s="9" t="s">
-        <v>30</v>
+        <v>135</v>
       </c>
       <c r="Y31" s="7"/>
     </row>
     <row r="35" spans="1:25">
       <c r="A35" s="4" t="s">
-        <v>156</v>
+        <v>67</v>
       </c>
     </row>
     <row r="36" spans="1:25">
@@ -10347,7 +10340,7 @@
         <v>2020</v>
       </c>
       <c r="Y36" s="6" t="s">
-        <v>28</v>
+        <v>133</v>
       </c>
     </row>
     <row r="37" spans="1:25">
@@ -10377,7 +10370,7 @@
       <c r="V37" s="12"/>
       <c r="W37" s="12"/>
       <c r="X37" s="9" t="s">
-        <v>30</v>
+        <v>135</v>
       </c>
       <c r="Y37" s="12">
         <v>0</v>
@@ -10410,7 +10403,7 @@
       <c r="V38" s="12"/>
       <c r="W38" s="12"/>
       <c r="X38" s="9" t="s">
-        <v>30</v>
+        <v>135</v>
       </c>
       <c r="Y38" s="12">
         <v>0</v>
@@ -10443,7 +10436,7 @@
       <c r="V39" s="12"/>
       <c r="W39" s="12"/>
       <c r="X39" s="9" t="s">
-        <v>30</v>
+        <v>135</v>
       </c>
       <c r="Y39" s="12">
         <v>0</v>
@@ -10476,7 +10469,7 @@
       <c r="V40" s="12"/>
       <c r="W40" s="12"/>
       <c r="X40" s="9" t="s">
-        <v>30</v>
+        <v>135</v>
       </c>
       <c r="Y40" s="12">
         <v>0</v>
@@ -10509,7 +10502,7 @@
       <c r="V41" s="12"/>
       <c r="W41" s="12"/>
       <c r="X41" s="9" t="s">
-        <v>30</v>
+        <v>135</v>
       </c>
       <c r="Y41" s="12">
         <v>0</v>
@@ -10517,7 +10510,7 @@
     </row>
     <row r="45" spans="1:25">
       <c r="A45" s="4" t="s">
-        <v>157</v>
+        <v>0</v>
       </c>
     </row>
     <row r="46" spans="1:25">
@@ -10585,12 +10578,12 @@
         <v>2020</v>
       </c>
       <c r="Y46" s="6" t="s">
-        <v>28</v>
+        <v>133</v>
       </c>
     </row>
     <row r="47" spans="1:25">
       <c r="B47" s="6" t="s">
-        <v>38</v>
+        <v>143</v>
       </c>
       <c r="C47" s="7"/>
       <c r="D47" s="7"/>
@@ -10618,13 +10611,13 @@
       <c r="V47" s="7"/>
       <c r="W47" s="7"/>
       <c r="X47" s="9" t="s">
-        <v>30</v>
+        <v>135</v>
       </c>
       <c r="Y47" s="7"/>
     </row>
     <row r="51" spans="1:25">
       <c r="A51" s="4" t="s">
-        <v>158</v>
+        <v>1</v>
       </c>
     </row>
     <row r="52" spans="1:25">
@@ -10692,7 +10685,7 @@
         <v>2020</v>
       </c>
       <c r="Y52" s="6" t="s">
-        <v>28</v>
+        <v>133</v>
       </c>
     </row>
     <row r="53" spans="1:25">
@@ -10750,7 +10743,7 @@
       <c r="V53" s="11"/>
       <c r="W53" s="11"/>
       <c r="X53" s="9" t="s">
-        <v>30</v>
+        <v>135</v>
       </c>
       <c r="Y53" s="11"/>
     </row>
@@ -10809,13 +10802,13 @@
       <c r="V54" s="11"/>
       <c r="W54" s="11"/>
       <c r="X54" s="9" t="s">
-        <v>30</v>
+        <v>135</v>
       </c>
       <c r="Y54" s="11"/>
     </row>
     <row r="58" spans="1:25">
       <c r="A58" s="4" t="s">
-        <v>159</v>
+        <v>2</v>
       </c>
     </row>
     <row r="59" spans="1:25">
@@ -10883,12 +10876,12 @@
         <v>2020</v>
       </c>
       <c r="Y59" s="6" t="s">
-        <v>28</v>
+        <v>133</v>
       </c>
     </row>
     <row r="60" spans="1:25">
       <c r="B60" s="6" t="s">
-        <v>38</v>
+        <v>143</v>
       </c>
       <c r="C60" s="12"/>
       <c r="D60" s="12"/>
@@ -10914,12 +10907,11 @@
       <c r="V60" s="12"/>
       <c r="W60" s="12"/>
       <c r="X60" s="9" t="s">
-        <v>30</v>
+        <v>135</v>
       </c>
       <c r="Y60" s="12"/>
     </row>
   </sheetData>
-  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
@@ -10944,7 +10936,7 @@
   <sheetData>
     <row r="1" spans="1:25">
       <c r="A1" s="4" t="s">
-        <v>160</v>
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:25">
@@ -11012,7 +11004,7 @@
         <v>2020</v>
       </c>
       <c r="Y2" s="6" t="s">
-        <v>28</v>
+        <v>133</v>
       </c>
     </row>
     <row r="3" spans="1:25">
@@ -11044,7 +11036,7 @@
       <c r="V3" s="7"/>
       <c r="W3" s="7"/>
       <c r="X3" s="9" t="s">
-        <v>30</v>
+        <v>135</v>
       </c>
       <c r="Y3" s="7"/>
     </row>
@@ -11077,7 +11069,7 @@
       <c r="V4" s="7"/>
       <c r="W4" s="7"/>
       <c r="X4" s="9" t="s">
-        <v>30</v>
+        <v>135</v>
       </c>
       <c r="Y4" s="7"/>
     </row>
@@ -11110,7 +11102,7 @@
       <c r="V5" s="7"/>
       <c r="W5" s="7"/>
       <c r="X5" s="9" t="s">
-        <v>30</v>
+        <v>135</v>
       </c>
       <c r="Y5" s="7"/>
     </row>
@@ -11143,7 +11135,7 @@
       <c r="V6" s="7"/>
       <c r="W6" s="7"/>
       <c r="X6" s="9" t="s">
-        <v>30</v>
+        <v>135</v>
       </c>
       <c r="Y6" s="7"/>
     </row>
@@ -11176,13 +11168,13 @@
       <c r="V7" s="7"/>
       <c r="W7" s="7"/>
       <c r="X7" s="9" t="s">
-        <v>30</v>
+        <v>135</v>
       </c>
       <c r="Y7" s="7"/>
     </row>
     <row r="11" spans="1:25">
       <c r="A11" s="4" t="s">
-        <v>161</v>
+        <v>4</v>
       </c>
     </row>
     <row r="12" spans="1:25">
@@ -11250,7 +11242,7 @@
         <v>2020</v>
       </c>
       <c r="Y12" s="6" t="s">
-        <v>28</v>
+        <v>133</v>
       </c>
     </row>
     <row r="13" spans="1:25">
@@ -11282,7 +11274,7 @@
       <c r="V13" s="7"/>
       <c r="W13" s="7"/>
       <c r="X13" s="9" t="s">
-        <v>30</v>
+        <v>135</v>
       </c>
       <c r="Y13" s="7"/>
     </row>
@@ -11315,7 +11307,7 @@
       <c r="V14" s="7"/>
       <c r="W14" s="7"/>
       <c r="X14" s="9" t="s">
-        <v>30</v>
+        <v>135</v>
       </c>
       <c r="Y14" s="7"/>
     </row>
@@ -11348,7 +11340,7 @@
       <c r="V15" s="7"/>
       <c r="W15" s="7"/>
       <c r="X15" s="9" t="s">
-        <v>30</v>
+        <v>135</v>
       </c>
       <c r="Y15" s="7"/>
     </row>
@@ -11381,7 +11373,7 @@
       <c r="V16" s="7"/>
       <c r="W16" s="7"/>
       <c r="X16" s="9" t="s">
-        <v>30</v>
+        <v>135</v>
       </c>
       <c r="Y16" s="7"/>
     </row>
@@ -11414,13 +11406,13 @@
       <c r="V17" s="7"/>
       <c r="W17" s="7"/>
       <c r="X17" s="9" t="s">
-        <v>30</v>
+        <v>135</v>
       </c>
       <c r="Y17" s="7"/>
     </row>
     <row r="21" spans="1:25">
       <c r="A21" s="4" t="s">
-        <v>162</v>
+        <v>5</v>
       </c>
     </row>
     <row r="22" spans="1:25">
@@ -11488,7 +11480,7 @@
         <v>2020</v>
       </c>
       <c r="Y22" s="6" t="s">
-        <v>28</v>
+        <v>133</v>
       </c>
     </row>
     <row r="23" spans="1:25">
@@ -11520,7 +11512,7 @@
       <c r="V23" s="7"/>
       <c r="W23" s="7"/>
       <c r="X23" s="9" t="s">
-        <v>30</v>
+        <v>135</v>
       </c>
       <c r="Y23" s="7"/>
     </row>
@@ -11553,7 +11545,7 @@
       <c r="V24" s="7"/>
       <c r="W24" s="7"/>
       <c r="X24" s="9" t="s">
-        <v>30</v>
+        <v>135</v>
       </c>
       <c r="Y24" s="7"/>
     </row>
@@ -11584,7 +11576,7 @@
       <c r="V25" s="7"/>
       <c r="W25" s="7"/>
       <c r="X25" s="9" t="s">
-        <v>30</v>
+        <v>135</v>
       </c>
       <c r="Y25" s="7"/>
     </row>
@@ -11615,7 +11607,7 @@
       <c r="V26" s="7"/>
       <c r="W26" s="7"/>
       <c r="X26" s="9" t="s">
-        <v>30</v>
+        <v>135</v>
       </c>
       <c r="Y26" s="7"/>
     </row>
@@ -11646,13 +11638,13 @@
       <c r="V27" s="7"/>
       <c r="W27" s="7"/>
       <c r="X27" s="9" t="s">
-        <v>30</v>
+        <v>135</v>
       </c>
       <c r="Y27" s="7"/>
     </row>
     <row r="31" spans="1:25">
       <c r="A31" s="4" t="s">
-        <v>163</v>
+        <v>6</v>
       </c>
     </row>
     <row r="32" spans="1:25">
@@ -11720,7 +11712,7 @@
         <v>2020</v>
       </c>
       <c r="Y32" s="6" t="s">
-        <v>28</v>
+        <v>133</v>
       </c>
     </row>
     <row r="33" spans="1:25">
@@ -11752,7 +11744,7 @@
       <c r="V33" s="12"/>
       <c r="W33" s="12"/>
       <c r="X33" s="9" t="s">
-        <v>30</v>
+        <v>135</v>
       </c>
       <c r="Y33" s="12"/>
     </row>
@@ -11785,7 +11777,7 @@
       <c r="V34" s="12"/>
       <c r="W34" s="12"/>
       <c r="X34" s="9" t="s">
-        <v>30</v>
+        <v>135</v>
       </c>
       <c r="Y34" s="12"/>
     </row>
@@ -11818,7 +11810,7 @@
       <c r="V35" s="12"/>
       <c r="W35" s="12"/>
       <c r="X35" s="9" t="s">
-        <v>30</v>
+        <v>135</v>
       </c>
       <c r="Y35" s="12"/>
     </row>
@@ -11851,7 +11843,7 @@
       <c r="V36" s="12"/>
       <c r="W36" s="12"/>
       <c r="X36" s="9" t="s">
-        <v>30</v>
+        <v>135</v>
       </c>
       <c r="Y36" s="12"/>
     </row>
@@ -11884,13 +11876,13 @@
       <c r="V37" s="12"/>
       <c r="W37" s="12"/>
       <c r="X37" s="9" t="s">
-        <v>30</v>
+        <v>135</v>
       </c>
       <c r="Y37" s="12"/>
     </row>
     <row r="41" spans="1:25">
       <c r="A41" s="4" t="s">
-        <v>74</v>
+        <v>80</v>
       </c>
     </row>
     <row r="42" spans="1:25">
@@ -11958,7 +11950,7 @@
         <v>2020</v>
       </c>
       <c r="Y42" s="6" t="s">
-        <v>28</v>
+        <v>133</v>
       </c>
     </row>
     <row r="43" spans="1:25">
@@ -11990,7 +11982,7 @@
       <c r="V43" s="12"/>
       <c r="W43" s="12"/>
       <c r="X43" s="9" t="s">
-        <v>30</v>
+        <v>135</v>
       </c>
       <c r="Y43" s="12"/>
     </row>
@@ -12023,7 +12015,7 @@
       <c r="V44" s="12"/>
       <c r="W44" s="12"/>
       <c r="X44" s="9" t="s">
-        <v>30</v>
+        <v>135</v>
       </c>
       <c r="Y44" s="12"/>
     </row>
@@ -12056,7 +12048,7 @@
       <c r="V45" s="12"/>
       <c r="W45" s="12"/>
       <c r="X45" s="9" t="s">
-        <v>30</v>
+        <v>135</v>
       </c>
       <c r="Y45" s="12"/>
     </row>
@@ -12089,7 +12081,7 @@
       <c r="V46" s="12"/>
       <c r="W46" s="12"/>
       <c r="X46" s="9" t="s">
-        <v>30</v>
+        <v>135</v>
       </c>
       <c r="Y46" s="12"/>
     </row>
@@ -12122,13 +12114,13 @@
       <c r="V47" s="12"/>
       <c r="W47" s="12"/>
       <c r="X47" s="9" t="s">
-        <v>30</v>
+        <v>135</v>
       </c>
       <c r="Y47" s="12"/>
     </row>
     <row r="51" spans="1:25">
       <c r="A51" s="4" t="s">
-        <v>75</v>
+        <v>81</v>
       </c>
     </row>
     <row r="52" spans="1:25">
@@ -12196,7 +12188,7 @@
         <v>2020</v>
       </c>
       <c r="Y52" s="6" t="s">
-        <v>28</v>
+        <v>133</v>
       </c>
     </row>
     <row r="53" spans="1:25">
@@ -12228,7 +12220,7 @@
       <c r="V53" s="12"/>
       <c r="W53" s="12"/>
       <c r="X53" s="9" t="s">
-        <v>30</v>
+        <v>135</v>
       </c>
       <c r="Y53" s="12"/>
     </row>
@@ -12261,7 +12253,7 @@
       <c r="V54" s="12"/>
       <c r="W54" s="12"/>
       <c r="X54" s="9" t="s">
-        <v>30</v>
+        <v>135</v>
       </c>
       <c r="Y54" s="12"/>
     </row>
@@ -12292,7 +12284,7 @@
       <c r="V55" s="12"/>
       <c r="W55" s="12"/>
       <c r="X55" s="9" t="s">
-        <v>30</v>
+        <v>135</v>
       </c>
       <c r="Y55" s="12">
         <v>0</v>
@@ -12325,7 +12317,7 @@
       <c r="V56" s="12"/>
       <c r="W56" s="12"/>
       <c r="X56" s="9" t="s">
-        <v>30</v>
+        <v>135</v>
       </c>
       <c r="Y56" s="12">
         <v>0</v>
@@ -12358,7 +12350,7 @@
       <c r="V57" s="12"/>
       <c r="W57" s="12"/>
       <c r="X57" s="9" t="s">
-        <v>30</v>
+        <v>135</v>
       </c>
       <c r="Y57" s="12">
         <v>0</v>
@@ -12366,7 +12358,7 @@
     </row>
     <row r="61" spans="1:25">
       <c r="A61" s="4" t="s">
-        <v>76</v>
+        <v>82</v>
       </c>
     </row>
     <row r="62" spans="1:25">
@@ -12434,7 +12426,7 @@
         <v>2020</v>
       </c>
       <c r="Y62" s="6" t="s">
-        <v>28</v>
+        <v>133</v>
       </c>
     </row>
     <row r="63" spans="1:25">
@@ -12466,7 +12458,7 @@
       <c r="V63" s="12"/>
       <c r="W63" s="12"/>
       <c r="X63" s="9" t="s">
-        <v>30</v>
+        <v>135</v>
       </c>
       <c r="Y63" s="12"/>
     </row>
@@ -12499,7 +12491,7 @@
       <c r="V64" s="12"/>
       <c r="W64" s="12"/>
       <c r="X64" s="9" t="s">
-        <v>30</v>
+        <v>135</v>
       </c>
       <c r="Y64" s="12"/>
     </row>
@@ -12532,12 +12524,11 @@
       <c r="V65" s="12"/>
       <c r="W65" s="12"/>
       <c r="X65" s="9" t="s">
-        <v>30</v>
+        <v>135</v>
       </c>
       <c r="Y65" s="12"/>
     </row>
   </sheetData>
-  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
@@ -12562,7 +12553,7 @@
   <sheetData>
     <row r="1" spans="1:25">
       <c r="A1" s="4" t="s">
-        <v>77</v>
+        <v>83</v>
       </c>
     </row>
     <row r="2" spans="1:25">
@@ -12630,7 +12621,7 @@
         <v>2020</v>
       </c>
       <c r="Y2" s="6" t="s">
-        <v>28</v>
+        <v>133</v>
       </c>
     </row>
     <row r="3" spans="1:25">
@@ -12662,7 +12653,7 @@
       <c r="V3" s="7"/>
       <c r="W3" s="7"/>
       <c r="X3" s="9" t="s">
-        <v>30</v>
+        <v>135</v>
       </c>
       <c r="Y3" s="7"/>
     </row>
@@ -12693,7 +12684,7 @@
       <c r="V4" s="7"/>
       <c r="W4" s="7"/>
       <c r="X4" s="9" t="s">
-        <v>30</v>
+        <v>135</v>
       </c>
       <c r="Y4" s="7">
         <v>0</v>
@@ -12728,7 +12719,7 @@
       <c r="V5" s="7"/>
       <c r="W5" s="7"/>
       <c r="X5" s="9" t="s">
-        <v>30</v>
+        <v>135</v>
       </c>
       <c r="Y5" s="7"/>
     </row>
@@ -12759,7 +12750,7 @@
       <c r="V6" s="7"/>
       <c r="W6" s="7"/>
       <c r="X6" s="9" t="s">
-        <v>30</v>
+        <v>135</v>
       </c>
       <c r="Y6" s="7">
         <v>0</v>
@@ -12792,7 +12783,7 @@
       <c r="V7" s="7"/>
       <c r="W7" s="7"/>
       <c r="X7" s="9" t="s">
-        <v>30</v>
+        <v>135</v>
       </c>
       <c r="Y7" s="7">
         <v>0</v>
@@ -12800,7 +12791,7 @@
     </row>
     <row r="11" spans="1:25">
       <c r="A11" s="4" t="s">
-        <v>78</v>
+        <v>84</v>
       </c>
     </row>
     <row r="12" spans="1:25">
@@ -12868,7 +12859,7 @@
         <v>2020</v>
       </c>
       <c r="Y12" s="6" t="s">
-        <v>28</v>
+        <v>133</v>
       </c>
     </row>
     <row r="13" spans="1:25">
@@ -12898,7 +12889,7 @@
       <c r="V13" s="12"/>
       <c r="W13" s="12"/>
       <c r="X13" s="9" t="s">
-        <v>30</v>
+        <v>135</v>
       </c>
       <c r="Y13" s="12">
         <v>0.2</v>
@@ -12931,7 +12922,7 @@
       <c r="V14" s="12"/>
       <c r="W14" s="12"/>
       <c r="X14" s="9" t="s">
-        <v>30</v>
+        <v>135</v>
       </c>
       <c r="Y14" s="12">
         <v>0</v>
@@ -12964,7 +12955,7 @@
       <c r="V15" s="12"/>
       <c r="W15" s="12"/>
       <c r="X15" s="9" t="s">
-        <v>30</v>
+        <v>135</v>
       </c>
       <c r="Y15" s="12">
         <v>0.2</v>
@@ -12997,7 +12988,7 @@
       <c r="V16" s="12"/>
       <c r="W16" s="12"/>
       <c r="X16" s="9" t="s">
-        <v>30</v>
+        <v>135</v>
       </c>
       <c r="Y16" s="12">
         <v>0</v>
@@ -13030,7 +13021,7 @@
       <c r="V17" s="12"/>
       <c r="W17" s="12"/>
       <c r="X17" s="9" t="s">
-        <v>30</v>
+        <v>135</v>
       </c>
       <c r="Y17" s="12">
         <v>0</v>
@@ -13038,7 +13029,7 @@
     </row>
     <row r="21" spans="1:25">
       <c r="A21" s="4" t="s">
-        <v>0</v>
+        <v>105</v>
       </c>
     </row>
     <row r="22" spans="1:25">
@@ -13106,12 +13097,12 @@
         <v>2020</v>
       </c>
       <c r="Y22" s="6" t="s">
-        <v>28</v>
+        <v>133</v>
       </c>
     </row>
     <row r="23" spans="1:25">
       <c r="B23" s="6" t="s">
-        <v>152</v>
+        <v>63</v>
       </c>
       <c r="C23" s="7"/>
       <c r="D23" s="7"/>
@@ -13135,14 +13126,13 @@
       <c r="V23" s="7"/>
       <c r="W23" s="7"/>
       <c r="X23" s="9" t="s">
-        <v>30</v>
+        <v>135</v>
       </c>
       <c r="Y23" s="7">
         <v>0</v>
       </c>
     </row>
   </sheetData>
-  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>

</xml_diff>